<commit_message>
Updated DU (late), created empty test cases document
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPM Project\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C340315-8251-4D8B-98D3-3327C20FCB27}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98102F71-2E5A-432A-8C88-83FAEA614160}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="64">
   <si>
     <t>Question</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>What will you do today?</t>
-  </si>
-  <si>
-    <t>Tee Yong</t>
   </si>
   <si>
     <t>Ngo Thanh Van (Christine)</t>
@@ -197,6 +194,33 @@
   </si>
   <si>
     <t>Update schedule, plan meeting content for tomorrow</t>
+  </si>
+  <si>
+    <t>Group meeting on schedule, milestones, and progress updates.</t>
+  </si>
+  <si>
+    <t>Plan my own milestones to complete the assigned tasks</t>
+  </si>
+  <si>
+    <t>Neo Tee Yong</t>
+  </si>
+  <si>
+    <t>Read through the codes committed by my teammates.</t>
+  </si>
+  <si>
+    <t>Group meeting on schedule, milestones, and progress updates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commit minutes </t>
+  </si>
+  <si>
+    <t>Conduct group meeting, set new expectations, rules and work methods as previous week was not as effective as expected</t>
+  </si>
+  <si>
+    <t>Update scheduling for the team, coordinate pair programming sessions and check through all existing management documents</t>
+  </si>
+  <si>
+    <t>Find tasks time consuming</t>
   </si>
 </sst>
 </file>
@@ -617,9 +641,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F36" sqref="F36"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -642,7 +666,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -712,7 +736,7 @@
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>7</v>
@@ -720,19 +744,19 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
@@ -743,19 +767,19 @@
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -766,24 +790,24 @@
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>7</v>
@@ -791,19 +815,19 @@
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -814,19 +838,19 @@
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -837,24 +861,24 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>7</v>
@@ -862,19 +886,19 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -885,19 +909,19 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -908,24 +932,24 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>7</v>
@@ -933,19 +957,19 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>32</v>
-      </c>
       <c r="G12" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -956,19 +980,19 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -979,24 +1003,24 @@
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>7</v>
@@ -1004,19 +1028,19 @@
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1027,19 +1051,19 @@
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1050,19 +1074,19 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -5024,9 +5048,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5049,7 +5073,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -5119,18 +5143,20 @@
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -5142,12 +5168,14 @@
         <v>12</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -5159,12 +5187,14 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -5172,18 +5202,20 @@
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
@@ -5195,12 +5227,14 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -5212,12 +5246,14 @@
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
@@ -5225,18 +5261,20 @@
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
@@ -5248,12 +5286,14 @@
         <v>8</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>58</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
@@ -5265,12 +5305,14 @@
         <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
@@ -5278,18 +5320,20 @@
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>61</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
@@ -5301,12 +5345,14 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
@@ -5318,12 +5364,14 @@
         <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
@@ -5331,18 +5379,20 @@
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
@@ -5354,12 +5404,14 @@
         <v>8</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>60</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
@@ -5371,12 +5423,14 @@
         <v>9</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>

</xml_diff>

<commit_message>
du for 3 Oct (Thurs)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6479CD27-6EAE-4A5C-85BB-7AD3E05AEE71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33D72F3-3D98-461F-BD67-92B13D2AA8C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6240" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="127">
   <si>
     <t>Question</t>
   </si>
@@ -397,6 +397,21 @@
   <si>
     <t>Met with  teammates before PM review, discussed with the group about the feedback from PM review</t>
   </si>
+  <si>
+    <t>Meeting with team to discuss the project in iteration 2</t>
+  </si>
+  <si>
+    <t>Pair Programming with lifu to do token verification</t>
+  </si>
+  <si>
+    <t>Meeting with team to discuss the project in iteration 2. Committed the minute of the meeting</t>
+  </si>
+  <si>
+    <t>Meet up with the team to discuss the project requirements in Interation 2.</t>
+  </si>
+  <si>
+    <t>Pair Programming with Tee Yong to do token verification</t>
+  </si>
 </sst>
 </file>
 
@@ -478,7 +493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -538,6 +553,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -864,21 +882,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -898,8 +916,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -940,7 +958,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -965,7 +983,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -988,7 +1006,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1011,7 +1029,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1036,7 +1054,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1059,7 +1077,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1082,7 +1100,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1107,7 +1125,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1130,7 +1148,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1153,7 +1171,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1178,7 +1196,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1201,7 +1219,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1224,7 +1242,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1249,7 +1267,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1272,7 +1290,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5255,7 +5273,7 @@
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+      <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5271,21 +5289,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5305,8 +5323,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5347,7 +5365,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5376,7 +5394,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5403,7 +5421,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5430,7 +5448,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5459,7 +5477,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5486,7 +5504,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5513,7 +5531,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5542,7 +5560,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5569,7 +5587,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5596,7 +5614,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5625,7 +5643,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5652,7 +5670,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5679,7 +5697,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5708,7 +5726,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5735,7 +5753,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9720,9 +9738,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9738,21 +9756,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9772,8 +9790,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9814,7 +9832,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9829,13 +9847,15 @@
       <c r="E3" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="24" t="s">
+        <v>122</v>
+      </c>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -9848,13 +9868,15 @@
       <c r="E4" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -9867,13 +9889,15 @@
       <c r="E5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -9888,13 +9912,15 @@
       <c r="E6" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="24" t="s">
+        <v>124</v>
+      </c>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -9907,13 +9933,15 @@
       <c r="E7" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -9926,13 +9954,15 @@
       <c r="E8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="25" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -9947,13 +9977,15 @@
       <c r="E9" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="24" t="s">
+        <v>125</v>
+      </c>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -9966,13 +9998,15 @@
       <c r="E10" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -9985,13 +10019,15 @@
       <c r="E11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="21"/>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
+      <c r="A12" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10006,13 +10042,15 @@
       <c r="E12" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="24" t="s">
+        <v>125</v>
+      </c>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10025,13 +10063,15 @@
       <c r="E13" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F13" s="21"/>
+      <c r="F13" s="24" t="s">
+        <v>126</v>
+      </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10044,13 +10084,15 @@
       <c r="E14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="21"/>
+      <c r="F14" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10065,13 +10107,15 @@
       <c r="E15" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="24" t="s">
+        <v>125</v>
+      </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10084,13 +10128,15 @@
       <c r="E16" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -10103,7 +10149,9 @@
       <c r="E17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>

</xml_diff>

<commit_message>
du for 4 Oct (Friday)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33D72F3-3D98-461F-BD67-92B13D2AA8C6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3970E66-A88C-4A35-9379-F187061C4D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6240" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="133">
   <si>
     <t>Question</t>
   </si>
@@ -412,6 +412,24 @@
   <si>
     <t>Pair Programming with Tee Yong to do token verification</t>
   </si>
+  <si>
+    <t>Pair Programming with lifu to do bootstrap verification</t>
+  </si>
+  <si>
+    <t>Pair Programming with tee yong for token verification</t>
+  </si>
+  <si>
+    <t>Pair Programming with tee yong for bootstrap verification</t>
+  </si>
+  <si>
+    <t>Pair Programming with Yu Liang for Add Bid function</t>
+  </si>
+  <si>
+    <t>Pair Programming with Christine for Add Bid function</t>
+  </si>
+  <si>
+    <t>Look at the schedule and plan accordingly</t>
+  </si>
 </sst>
 </file>
 
@@ -493,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -553,6 +571,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -882,21 +903,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -916,8 +937,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -958,7 +979,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -983,7 +1004,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1006,7 +1027,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1050,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1054,7 +1075,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1077,7 +1098,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1100,7 +1121,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1125,7 +1146,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1148,7 +1169,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1192,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1196,7 +1217,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1240,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1242,7 +1263,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1267,7 +1288,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1311,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5289,21 +5310,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5323,8 +5344,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5365,7 +5386,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5394,7 +5415,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5421,7 +5442,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5448,7 +5469,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5477,7 +5498,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5504,7 +5525,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5531,7 +5552,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5560,7 +5581,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5587,7 +5608,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5614,7 +5635,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5643,7 +5664,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5670,7 +5691,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5697,7 +5718,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5726,7 +5747,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5753,7 +5774,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9739,8 +9760,8 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9756,21 +9777,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9790,8 +9811,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9832,7 +9853,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9850,12 +9871,14 @@
       <c r="F3" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="25" t="s">
+        <v>123</v>
+      </c>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -9871,12 +9894,14 @@
       <c r="F4" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="25" t="s">
+        <v>127</v>
+      </c>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -9892,12 +9917,14 @@
       <c r="F5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="21"/>
+      <c r="G5" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -9915,12 +9942,14 @@
       <c r="F6" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="21"/>
+      <c r="G6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -9936,12 +9965,14 @@
       <c r="F7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="21"/>
+      <c r="G7" s="25" t="s">
+        <v>130</v>
+      </c>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -9957,12 +9988,14 @@
       <c r="F8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -9980,12 +10013,14 @@
       <c r="F9" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="21"/>
+      <c r="G9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10001,12 +10036,14 @@
       <c r="F10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="21"/>
+      <c r="G10" s="25" t="s">
+        <v>131</v>
+      </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10022,12 +10059,14 @@
       <c r="F11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10045,12 +10084,14 @@
       <c r="F12" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="21"/>
+      <c r="G12" s="25" t="s">
+        <v>128</v>
+      </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10066,12 +10107,14 @@
       <c r="F13" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="21"/>
+      <c r="G13" s="25" t="s">
+        <v>129</v>
+      </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10087,12 +10130,14 @@
       <c r="F14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="26" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10110,12 +10155,14 @@
       <c r="F15" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
+      <c r="A16" s="27"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10131,12 +10178,14 @@
       <c r="F16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="21" t="s">
+        <v>132</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -10152,7 +10201,9 @@
       <c r="F17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
     </row>

</xml_diff>

<commit_message>
du for 5 Oct (Sat)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3970E66-A88C-4A35-9379-F187061C4D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2145BEC-35A4-493C-87DF-566968A544A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="141">
   <si>
     <t>Question</t>
   </si>
@@ -430,6 +430,30 @@
   <si>
     <t>Look at the schedule and plan accordingly</t>
   </si>
+  <si>
+    <t>Continue Pair Programming with Christine for Add Bid function &amp; Meeting up with the team to update on our progress and discuss if we faced and difficulties</t>
+  </si>
+  <si>
+    <t>Meet up with team to discuss on progress</t>
+  </si>
+  <si>
+    <t>Pair Programming with tee yong to do bootstrap verification</t>
+  </si>
+  <si>
+    <t>Team meeting to discuss on progression</t>
+  </si>
+  <si>
+    <t>Pair Programming with Yu Liang to do Add Bid verification</t>
+  </si>
+  <si>
+    <t>Team meeting to discuss on progression &amp; continue pair programming meet up with Yu Liang to do Add Bid function</t>
+  </si>
+  <si>
+    <t>Looked at the schedule and made some planning</t>
+  </si>
+  <si>
+    <t>Have a team meeting to discuss on our progress and update schedule accordingly</t>
+  </si>
 </sst>
 </file>
 
@@ -511,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -571,6 +595,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -903,21 +930,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -937,8 +964,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -979,7 +1006,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1004,7 +1031,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1027,7 +1054,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +1077,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1075,7 +1102,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1098,7 +1125,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1121,7 +1148,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1146,7 +1173,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1196,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +1219,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1217,7 +1244,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1240,7 +1267,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1290,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1288,7 +1315,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1311,7 +1338,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5293,7 +5320,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -5310,21 +5337,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5344,8 +5371,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5386,7 +5413,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5415,7 +5442,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5442,7 +5469,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5469,7 +5496,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5498,7 +5525,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5525,7 +5552,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5552,7 +5579,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5581,7 +5608,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5608,7 +5635,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5635,7 +5662,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5664,7 +5691,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5691,7 +5718,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5718,7 +5745,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5747,7 +5774,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5774,7 +5801,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9760,8 +9787,8 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G16" sqref="G16"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9777,21 +9804,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9811,8 +9838,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9853,7 +9880,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9874,11 +9901,13 @@
       <c r="G3" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="26" t="s">
+        <v>127</v>
+      </c>
       <c r="I3" s="21"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -9897,11 +9926,13 @@
       <c r="G4" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="26" t="s">
+        <v>134</v>
+      </c>
       <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -9920,11 +9951,13 @@
       <c r="G5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="I5" s="21"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="27" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -9945,11 +9978,13 @@
       <c r="G6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="26" t="s">
+        <v>137</v>
+      </c>
       <c r="I6" s="21"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -9968,11 +10003,13 @@
       <c r="G7" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="26" t="s">
+        <v>138</v>
+      </c>
       <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -9991,11 +10028,13 @@
       <c r="G8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="I8" s="21"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="27" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10016,11 +10055,13 @@
       <c r="G9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="26" t="s">
+        <v>131</v>
+      </c>
       <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10039,11 +10080,13 @@
       <c r="G10" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="26" t="s">
+        <v>133</v>
+      </c>
       <c r="I10" s="21"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10062,11 +10105,13 @@
       <c r="G11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="21"/>
+      <c r="H11" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="I11" s="21"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10087,11 +10132,13 @@
       <c r="G12" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="26" t="s">
+        <v>135</v>
+      </c>
       <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10110,11 +10157,13 @@
       <c r="G13" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="26" t="s">
+        <v>136</v>
+      </c>
       <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10133,11 +10182,13 @@
       <c r="G14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="21"/>
+      <c r="H14" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="27" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10158,11 +10209,13 @@
       <c r="G15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="21" t="s">
+        <v>139</v>
+      </c>
       <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10181,11 +10234,13 @@
       <c r="G16" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H16" s="21" t="s">
+        <v>140</v>
+      </c>
       <c r="I16" s="21"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -10204,7 +10259,9 @@
       <c r="G17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="21"/>
+      <c r="H17" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="I17" s="21"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
du for 6 Oct (Sun)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2145BEC-35A4-493C-87DF-566968A544A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87438153-B73F-4E91-A09C-20278C4B1978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="146">
   <si>
     <t>Question</t>
   </si>
@@ -453,6 +453,21 @@
   </si>
   <si>
     <t>Have a team meeting to discuss on our progress and update schedule accordingly</t>
+  </si>
+  <si>
+    <t>Meeting with team to update progress, tested bootstrap with teeyong and debugged accordingly</t>
+  </si>
+  <si>
+    <t>Meeting with team to update progress, tested bootstrap with Lifu and debugged accordingly</t>
+  </si>
+  <si>
+    <t>Continue Pair Programming with Yu Liang for Add Bid function &amp; Meeting up with the team to update on our progress and discuss if we faced and difficulties</t>
+  </si>
+  <si>
+    <t>Continue updating the schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting up with the team to check on everyone's progress and ensure that our schedule is going well </t>
   </si>
 </sst>
 </file>
@@ -535,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -595,6 +610,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -912,8 +930,8 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
@@ -930,21 +948,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -964,8 +982,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1006,7 +1024,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1031,7 +1049,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1054,7 +1072,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1077,7 +1095,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1102,7 +1120,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1125,7 +1143,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1148,7 +1166,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1173,7 +1191,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1196,7 +1214,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1219,7 +1237,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1244,7 +1262,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1285,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1308,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1315,7 +1333,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1338,7 +1356,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5337,21 +5355,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5371,8 +5389,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5413,7 +5431,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5442,7 +5460,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5469,7 +5487,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5496,7 +5514,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5525,7 +5543,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5552,7 +5570,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5579,7 +5597,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5608,7 +5626,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5635,7 +5653,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5662,7 +5680,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5691,7 +5709,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5718,7 +5736,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5745,7 +5763,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5774,7 +5792,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5801,7 +5819,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9788,7 +9806,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I17" sqref="I17"/>
+      <selection pane="topRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9804,21 +9822,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9838,8 +9856,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9880,7 +9898,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9904,10 +9922,12 @@
       <c r="H3" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="27" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -9929,10 +9949,12 @@
       <c r="H4" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -9954,10 +9976,12 @@
       <c r="H5" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="21"/>
+      <c r="I5" s="21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="28" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -9981,10 +10005,12 @@
       <c r="H6" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="27" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10006,10 +10032,12 @@
       <c r="H7" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10031,10 +10059,12 @@
       <c r="H8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10058,10 +10088,12 @@
       <c r="H9" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="I9" s="21"/>
+      <c r="I9" s="27" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10083,10 +10115,12 @@
       <c r="H10" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10108,10 +10142,12 @@
       <c r="H11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="21"/>
+      <c r="I11" s="21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10135,10 +10171,12 @@
       <c r="H12" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="I12" s="21"/>
+      <c r="I12" s="27" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10160,10 +10198,12 @@
       <c r="H13" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="I13" s="21"/>
+      <c r="I13" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10185,10 +10225,12 @@
       <c r="H14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="21"/>
+      <c r="I14" s="27" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10212,10 +10254,12 @@
       <c r="H15" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="I15" s="21"/>
+      <c r="I15" s="21" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10237,10 +10281,12 @@
       <c r="H16" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="I16" s="21"/>
+      <c r="I16" s="21" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -10262,7 +10308,9 @@
       <c r="H17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="21"/>
+      <c r="I17" s="21" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>

</xml_diff>

<commit_message>
du for 7 Oct (Mon)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87438153-B73F-4E91-A09C-20278C4B1978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDB683E-9DDA-4A63-B609-D80092B2ACDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
     <sheet name="Week 6" sheetId="6" r:id="rId2"/>
     <sheet name="Week 7" sheetId="7" r:id="rId3"/>
+    <sheet name="Week 8" sheetId="9" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="149">
   <si>
     <t>Question</t>
   </si>
@@ -469,6 +470,15 @@
   <si>
     <t xml:space="preserve">Meeting up with the team to check on everyone's progress and ensure that our schedule is going well </t>
   </si>
+  <si>
+    <t>Revise &amp; review php content, prepare for pair programming sessions during the recess week</t>
+  </si>
+  <si>
+    <t>Review the codes and prepare for continued pair programming on Add Bids function</t>
+  </si>
+  <si>
+    <t>Updated the schedule</t>
+  </si>
 </sst>
 </file>
 
@@ -550,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -634,6 +644,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -643,6 +662,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -925,7 +950,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C028D80-9818-4EA5-A3B1-42DA8998D09F}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z1001"/>
@@ -948,21 +973,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -982,8 +1007,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1024,7 +1049,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1049,7 +1074,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1072,7 +1097,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1095,7 +1120,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1120,7 +1145,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1143,7 +1168,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1166,7 +1191,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1191,7 +1216,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1214,7 +1239,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1262,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1262,7 +1287,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1285,7 +1310,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1333,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1333,7 +1358,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1381,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5332,7 +5357,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81166FA-1AD0-4E00-A496-37DA11C7D39D}">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z1001"/>
@@ -5355,21 +5380,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5389,8 +5414,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5431,7 +5456,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5460,7 +5485,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5487,7 +5512,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5514,7 +5539,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5543,7 +5568,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5570,7 +5595,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5597,7 +5622,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5626,7 +5651,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5653,7 +5678,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5680,7 +5705,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5709,7 +5734,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5736,7 +5761,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5763,7 +5788,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5792,7 +5817,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5819,7 +5844,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9799,14 +9824,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1AEA77-0749-462C-BEDD-F4E195366FF6}">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I16" sqref="I16"/>
+      <selection pane="topRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9822,21 +9847,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9856,8 +9881,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9898,7 +9923,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9927,7 +9952,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -9954,7 +9979,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="32"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -9981,7 +10006,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10010,7 +10035,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10037,7 +10062,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10064,7 +10089,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10093,7 +10118,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10120,7 +10145,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10147,7 +10172,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10176,7 +10201,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10203,7 +10228,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10230,7 +10255,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10259,7 +10284,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10286,7 +10311,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -10311,6 +10336,4293 @@
       <c r="I17" s="21" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="15"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="15"/>
+    </row>
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="15"/>
+    </row>
+    <row r="33" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="15"/>
+    </row>
+    <row r="34" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="15"/>
+    </row>
+    <row r="37" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="15"/>
+    </row>
+    <row r="38" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="15"/>
+    </row>
+    <row r="39" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="15"/>
+    </row>
+    <row r="41" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="15"/>
+    </row>
+    <row r="43" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="15"/>
+    </row>
+    <row r="44" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="15"/>
+    </row>
+    <row r="45" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="15"/>
+    </row>
+    <row r="46" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="15"/>
+    </row>
+    <row r="47" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="15"/>
+    </row>
+    <row r="48" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="15"/>
+    </row>
+    <row r="49" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="15"/>
+    </row>
+    <row r="50" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="15"/>
+    </row>
+    <row r="51" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="15"/>
+    </row>
+    <row r="52" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="18"/>
+      <c r="B52" s="15"/>
+    </row>
+    <row r="53" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="18"/>
+      <c r="B53" s="15"/>
+    </row>
+    <row r="54" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="18"/>
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="18"/>
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="18"/>
+      <c r="B56" s="15"/>
+    </row>
+    <row r="57" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="18"/>
+      <c r="B57" s="15"/>
+    </row>
+    <row r="58" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="15"/>
+    </row>
+    <row r="59" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="15"/>
+    </row>
+    <row r="60" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="18"/>
+      <c r="B60" s="15"/>
+    </row>
+    <row r="61" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="18"/>
+      <c r="B61" s="15"/>
+    </row>
+    <row r="62" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="18"/>
+      <c r="B62" s="15"/>
+    </row>
+    <row r="63" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="18"/>
+      <c r="B63" s="15"/>
+    </row>
+    <row r="64" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="18"/>
+      <c r="B64" s="15"/>
+    </row>
+    <row r="65" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="18"/>
+      <c r="B65" s="15"/>
+    </row>
+    <row r="66" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="18"/>
+      <c r="B66" s="15"/>
+    </row>
+    <row r="67" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="18"/>
+      <c r="B67" s="15"/>
+    </row>
+    <row r="68" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="18"/>
+      <c r="B68" s="15"/>
+    </row>
+    <row r="69" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="18"/>
+      <c r="B69" s="15"/>
+    </row>
+    <row r="70" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="18"/>
+      <c r="B70" s="15"/>
+    </row>
+    <row r="71" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
+      <c r="B71" s="15"/>
+    </row>
+    <row r="72" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="18"/>
+      <c r="B72" s="15"/>
+    </row>
+    <row r="73" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="18"/>
+      <c r="B73" s="15"/>
+    </row>
+    <row r="74" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="18"/>
+      <c r="B74" s="15"/>
+    </row>
+    <row r="75" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
+      <c r="B75" s="15"/>
+    </row>
+    <row r="76" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
+      <c r="B76" s="15"/>
+    </row>
+    <row r="77" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="18"/>
+      <c r="B77" s="15"/>
+    </row>
+    <row r="78" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="18"/>
+      <c r="B78" s="15"/>
+    </row>
+    <row r="79" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="18"/>
+      <c r="B79" s="15"/>
+    </row>
+    <row r="80" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="18"/>
+      <c r="B80" s="15"/>
+    </row>
+    <row r="81" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="18"/>
+      <c r="B81" s="15"/>
+    </row>
+    <row r="82" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="18"/>
+      <c r="B82" s="15"/>
+    </row>
+    <row r="83" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="18"/>
+      <c r="B83" s="15"/>
+    </row>
+    <row r="84" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="18"/>
+      <c r="B84" s="15"/>
+    </row>
+    <row r="85" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="18"/>
+      <c r="B85" s="15"/>
+    </row>
+    <row r="86" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="18"/>
+      <c r="B86" s="15"/>
+    </row>
+    <row r="87" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="18"/>
+      <c r="B87" s="15"/>
+    </row>
+    <row r="88" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="18"/>
+      <c r="B88" s="15"/>
+    </row>
+    <row r="89" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="18"/>
+      <c r="B89" s="15"/>
+    </row>
+    <row r="90" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="18"/>
+      <c r="B90" s="15"/>
+    </row>
+    <row r="91" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="18"/>
+      <c r="B91" s="15"/>
+    </row>
+    <row r="92" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="18"/>
+      <c r="B92" s="15"/>
+    </row>
+    <row r="93" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="18"/>
+      <c r="B93" s="15"/>
+    </row>
+    <row r="94" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="18"/>
+      <c r="B94" s="15"/>
+    </row>
+    <row r="95" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="18"/>
+      <c r="B95" s="15"/>
+    </row>
+    <row r="96" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="18"/>
+      <c r="B96" s="15"/>
+    </row>
+    <row r="97" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="18"/>
+      <c r="B97" s="15"/>
+    </row>
+    <row r="98" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="18"/>
+      <c r="B98" s="15"/>
+    </row>
+    <row r="99" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="18"/>
+      <c r="B99" s="15"/>
+    </row>
+    <row r="100" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="18"/>
+      <c r="B100" s="15"/>
+    </row>
+    <row r="101" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="18"/>
+      <c r="B101" s="15"/>
+    </row>
+    <row r="102" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="18"/>
+      <c r="B102" s="15"/>
+    </row>
+    <row r="103" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="18"/>
+      <c r="B103" s="15"/>
+    </row>
+    <row r="104" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="18"/>
+      <c r="B104" s="15"/>
+    </row>
+    <row r="105" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="18"/>
+      <c r="B105" s="15"/>
+    </row>
+    <row r="106" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="18"/>
+      <c r="B106" s="15"/>
+    </row>
+    <row r="107" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="18"/>
+      <c r="B107" s="15"/>
+    </row>
+    <row r="108" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="18"/>
+      <c r="B108" s="15"/>
+    </row>
+    <row r="109" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="18"/>
+      <c r="B109" s="15"/>
+    </row>
+    <row r="110" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="18"/>
+      <c r="B110" s="15"/>
+    </row>
+    <row r="111" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="18"/>
+      <c r="B111" s="15"/>
+    </row>
+    <row r="112" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="18"/>
+      <c r="B112" s="15"/>
+    </row>
+    <row r="113" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="18"/>
+      <c r="B113" s="15"/>
+    </row>
+    <row r="114" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="18"/>
+      <c r="B114" s="15"/>
+    </row>
+    <row r="115" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="18"/>
+      <c r="B115" s="15"/>
+    </row>
+    <row r="116" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="18"/>
+      <c r="B116" s="15"/>
+    </row>
+    <row r="117" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="18"/>
+      <c r="B117" s="15"/>
+    </row>
+    <row r="118" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="18"/>
+      <c r="B118" s="15"/>
+    </row>
+    <row r="119" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="18"/>
+      <c r="B119" s="15"/>
+    </row>
+    <row r="120" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="18"/>
+      <c r="B120" s="15"/>
+    </row>
+    <row r="121" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="18"/>
+      <c r="B121" s="15"/>
+    </row>
+    <row r="122" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="18"/>
+      <c r="B122" s="15"/>
+    </row>
+    <row r="123" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="18"/>
+      <c r="B123" s="15"/>
+    </row>
+    <row r="124" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="18"/>
+      <c r="B124" s="15"/>
+    </row>
+    <row r="125" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="18"/>
+      <c r="B125" s="15"/>
+    </row>
+    <row r="126" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="18"/>
+      <c r="B126" s="15"/>
+    </row>
+    <row r="127" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="18"/>
+      <c r="B127" s="15"/>
+    </row>
+    <row r="128" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="18"/>
+      <c r="B128" s="15"/>
+    </row>
+    <row r="129" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="18"/>
+      <c r="B129" s="15"/>
+    </row>
+    <row r="130" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="18"/>
+      <c r="B130" s="15"/>
+    </row>
+    <row r="131" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="18"/>
+      <c r="B131" s="15"/>
+    </row>
+    <row r="132" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="18"/>
+      <c r="B132" s="15"/>
+    </row>
+    <row r="133" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="18"/>
+      <c r="B133" s="15"/>
+    </row>
+    <row r="134" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="18"/>
+      <c r="B134" s="15"/>
+    </row>
+    <row r="135" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="18"/>
+      <c r="B135" s="15"/>
+    </row>
+    <row r="136" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="18"/>
+      <c r="B136" s="15"/>
+    </row>
+    <row r="137" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="18"/>
+      <c r="B137" s="15"/>
+    </row>
+    <row r="138" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="18"/>
+      <c r="B138" s="15"/>
+    </row>
+    <row r="139" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="18"/>
+      <c r="B139" s="15"/>
+    </row>
+    <row r="140" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="18"/>
+      <c r="B140" s="15"/>
+    </row>
+    <row r="141" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="18"/>
+      <c r="B141" s="15"/>
+    </row>
+    <row r="142" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="18"/>
+      <c r="B142" s="15"/>
+    </row>
+    <row r="143" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="18"/>
+      <c r="B143" s="15"/>
+    </row>
+    <row r="144" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="18"/>
+      <c r="B144" s="15"/>
+    </row>
+    <row r="145" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="18"/>
+      <c r="B145" s="15"/>
+    </row>
+    <row r="146" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="18"/>
+      <c r="B146" s="15"/>
+    </row>
+    <row r="147" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="18"/>
+      <c r="B147" s="15"/>
+    </row>
+    <row r="148" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="18"/>
+      <c r="B148" s="15"/>
+    </row>
+    <row r="149" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="18"/>
+      <c r="B149" s="15"/>
+    </row>
+    <row r="150" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="18"/>
+      <c r="B150" s="15"/>
+    </row>
+    <row r="151" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="18"/>
+      <c r="B151" s="15"/>
+    </row>
+    <row r="152" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="18"/>
+      <c r="B152" s="15"/>
+    </row>
+    <row r="153" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="18"/>
+      <c r="B153" s="15"/>
+    </row>
+    <row r="154" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="18"/>
+      <c r="B154" s="15"/>
+    </row>
+    <row r="155" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="18"/>
+      <c r="B155" s="15"/>
+    </row>
+    <row r="156" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A156" s="18"/>
+      <c r="B156" s="15"/>
+    </row>
+    <row r="157" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A157" s="18"/>
+      <c r="B157" s="15"/>
+    </row>
+    <row r="158" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A158" s="18"/>
+      <c r="B158" s="15"/>
+    </row>
+    <row r="159" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A159" s="18"/>
+      <c r="B159" s="15"/>
+    </row>
+    <row r="160" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A160" s="18"/>
+      <c r="B160" s="15"/>
+    </row>
+    <row r="161" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A161" s="18"/>
+      <c r="B161" s="15"/>
+    </row>
+    <row r="162" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A162" s="18"/>
+      <c r="B162" s="15"/>
+    </row>
+    <row r="163" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A163" s="18"/>
+      <c r="B163" s="15"/>
+    </row>
+    <row r="164" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A164" s="18"/>
+      <c r="B164" s="15"/>
+    </row>
+    <row r="165" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A165" s="18"/>
+      <c r="B165" s="15"/>
+    </row>
+    <row r="166" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A166" s="18"/>
+      <c r="B166" s="15"/>
+    </row>
+    <row r="167" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A167" s="18"/>
+      <c r="B167" s="15"/>
+    </row>
+    <row r="168" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A168" s="18"/>
+      <c r="B168" s="15"/>
+    </row>
+    <row r="169" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A169" s="18"/>
+      <c r="B169" s="15"/>
+    </row>
+    <row r="170" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A170" s="18"/>
+      <c r="B170" s="15"/>
+    </row>
+    <row r="171" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A171" s="18"/>
+      <c r="B171" s="15"/>
+    </row>
+    <row r="172" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A172" s="18"/>
+      <c r="B172" s="15"/>
+    </row>
+    <row r="173" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A173" s="18"/>
+      <c r="B173" s="15"/>
+    </row>
+    <row r="174" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A174" s="18"/>
+      <c r="B174" s="15"/>
+    </row>
+    <row r="175" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A175" s="18"/>
+      <c r="B175" s="15"/>
+    </row>
+    <row r="176" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A176" s="18"/>
+      <c r="B176" s="15"/>
+    </row>
+    <row r="177" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A177" s="18"/>
+      <c r="B177" s="15"/>
+    </row>
+    <row r="178" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A178" s="18"/>
+      <c r="B178" s="15"/>
+    </row>
+    <row r="179" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A179" s="18"/>
+      <c r="B179" s="15"/>
+    </row>
+    <row r="180" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A180" s="18"/>
+      <c r="B180" s="15"/>
+    </row>
+    <row r="181" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A181" s="18"/>
+      <c r="B181" s="15"/>
+    </row>
+    <row r="182" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A182" s="18"/>
+      <c r="B182" s="15"/>
+    </row>
+    <row r="183" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A183" s="18"/>
+      <c r="B183" s="15"/>
+    </row>
+    <row r="184" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A184" s="18"/>
+      <c r="B184" s="15"/>
+    </row>
+    <row r="185" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A185" s="18"/>
+      <c r="B185" s="15"/>
+    </row>
+    <row r="186" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A186" s="18"/>
+      <c r="B186" s="15"/>
+    </row>
+    <row r="187" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A187" s="18"/>
+      <c r="B187" s="15"/>
+    </row>
+    <row r="188" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A188" s="18"/>
+      <c r="B188" s="15"/>
+    </row>
+    <row r="189" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A189" s="18"/>
+      <c r="B189" s="15"/>
+    </row>
+    <row r="190" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A190" s="18"/>
+      <c r="B190" s="15"/>
+    </row>
+    <row r="191" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A191" s="18"/>
+      <c r="B191" s="15"/>
+    </row>
+    <row r="192" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A192" s="18"/>
+      <c r="B192" s="15"/>
+    </row>
+    <row r="193" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A193" s="18"/>
+      <c r="B193" s="15"/>
+    </row>
+    <row r="194" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A194" s="18"/>
+      <c r="B194" s="15"/>
+    </row>
+    <row r="195" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A195" s="18"/>
+      <c r="B195" s="15"/>
+    </row>
+    <row r="196" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A196" s="18"/>
+      <c r="B196" s="15"/>
+    </row>
+    <row r="197" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A197" s="18"/>
+      <c r="B197" s="15"/>
+    </row>
+    <row r="198" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A198" s="18"/>
+      <c r="B198" s="15"/>
+    </row>
+    <row r="199" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A199" s="18"/>
+      <c r="B199" s="15"/>
+    </row>
+    <row r="200" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A200" s="18"/>
+      <c r="B200" s="15"/>
+    </row>
+    <row r="201" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A201" s="18"/>
+      <c r="B201" s="15"/>
+    </row>
+    <row r="202" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A202" s="18"/>
+      <c r="B202" s="15"/>
+    </row>
+    <row r="203" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A203" s="18"/>
+      <c r="B203" s="15"/>
+    </row>
+    <row r="204" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A204" s="18"/>
+      <c r="B204" s="15"/>
+    </row>
+    <row r="205" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A205" s="18"/>
+      <c r="B205" s="15"/>
+    </row>
+    <row r="206" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A206" s="18"/>
+      <c r="B206" s="15"/>
+    </row>
+    <row r="207" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A207" s="18"/>
+      <c r="B207" s="15"/>
+    </row>
+    <row r="208" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A208" s="18"/>
+      <c r="B208" s="15"/>
+    </row>
+    <row r="209" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A209" s="18"/>
+      <c r="B209" s="15"/>
+    </row>
+    <row r="210" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A210" s="18"/>
+      <c r="B210" s="15"/>
+    </row>
+    <row r="211" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A211" s="18"/>
+      <c r="B211" s="15"/>
+    </row>
+    <row r="212" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A212" s="18"/>
+      <c r="B212" s="15"/>
+    </row>
+    <row r="213" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A213" s="18"/>
+      <c r="B213" s="15"/>
+    </row>
+    <row r="214" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A214" s="18"/>
+      <c r="B214" s="15"/>
+    </row>
+    <row r="215" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A215" s="18"/>
+      <c r="B215" s="15"/>
+    </row>
+    <row r="216" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A216" s="18"/>
+      <c r="B216" s="15"/>
+    </row>
+    <row r="217" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A217" s="18"/>
+      <c r="B217" s="15"/>
+    </row>
+    <row r="218" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A218" s="18"/>
+      <c r="B218" s="15"/>
+    </row>
+    <row r="219" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A219" s="18"/>
+      <c r="B219" s="15"/>
+    </row>
+    <row r="220" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A220" s="18"/>
+      <c r="B220" s="15"/>
+    </row>
+    <row r="221" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A221" s="18"/>
+      <c r="B221" s="15"/>
+    </row>
+    <row r="222" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A222" s="18"/>
+      <c r="B222" s="15"/>
+    </row>
+    <row r="223" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A223" s="18"/>
+      <c r="B223" s="15"/>
+    </row>
+    <row r="224" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A224" s="18"/>
+      <c r="B224" s="15"/>
+    </row>
+    <row r="225" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A225" s="18"/>
+      <c r="B225" s="15"/>
+    </row>
+    <row r="226" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A226" s="18"/>
+      <c r="B226" s="15"/>
+    </row>
+    <row r="227" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A227" s="18"/>
+      <c r="B227" s="15"/>
+    </row>
+    <row r="228" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A228" s="18"/>
+      <c r="B228" s="15"/>
+    </row>
+    <row r="229" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A229" s="18"/>
+      <c r="B229" s="15"/>
+    </row>
+    <row r="230" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A230" s="18"/>
+      <c r="B230" s="15"/>
+    </row>
+    <row r="231" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A231" s="18"/>
+      <c r="B231" s="15"/>
+    </row>
+    <row r="232" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A232" s="18"/>
+      <c r="B232" s="15"/>
+    </row>
+    <row r="233" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A233" s="18"/>
+      <c r="B233" s="15"/>
+    </row>
+    <row r="234" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A234" s="18"/>
+      <c r="B234" s="15"/>
+    </row>
+    <row r="235" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A235" s="18"/>
+      <c r="B235" s="15"/>
+    </row>
+    <row r="236" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A236" s="18"/>
+      <c r="B236" s="15"/>
+    </row>
+    <row r="237" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A237" s="18"/>
+      <c r="B237" s="15"/>
+    </row>
+    <row r="238" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A238" s="18"/>
+      <c r="B238" s="15"/>
+    </row>
+    <row r="239" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A239" s="18"/>
+      <c r="B239" s="15"/>
+    </row>
+    <row r="240" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A240" s="18"/>
+      <c r="B240" s="15"/>
+    </row>
+    <row r="241" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A241" s="18"/>
+      <c r="B241" s="15"/>
+    </row>
+    <row r="242" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A242" s="18"/>
+      <c r="B242" s="15"/>
+    </row>
+    <row r="243" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A243" s="18"/>
+      <c r="B243" s="15"/>
+    </row>
+    <row r="244" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A244" s="18"/>
+      <c r="B244" s="15"/>
+    </row>
+    <row r="245" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A245" s="18"/>
+      <c r="B245" s="15"/>
+    </row>
+    <row r="246" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A246" s="18"/>
+      <c r="B246" s="15"/>
+    </row>
+    <row r="247" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A247" s="18"/>
+      <c r="B247" s="15"/>
+    </row>
+    <row r="248" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A248" s="18"/>
+      <c r="B248" s="15"/>
+    </row>
+    <row r="249" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A249" s="18"/>
+      <c r="B249" s="15"/>
+    </row>
+    <row r="250" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A250" s="18"/>
+      <c r="B250" s="15"/>
+    </row>
+    <row r="251" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A251" s="18"/>
+      <c r="B251" s="15"/>
+    </row>
+    <row r="252" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A252" s="18"/>
+      <c r="B252" s="15"/>
+    </row>
+    <row r="253" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A253" s="18"/>
+      <c r="B253" s="15"/>
+    </row>
+    <row r="254" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A254" s="18"/>
+      <c r="B254" s="15"/>
+    </row>
+    <row r="255" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A255" s="18"/>
+      <c r="B255" s="15"/>
+    </row>
+    <row r="256" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A256" s="18"/>
+      <c r="B256" s="15"/>
+    </row>
+    <row r="257" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A257" s="18"/>
+      <c r="B257" s="15"/>
+    </row>
+    <row r="258" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A258" s="18"/>
+      <c r="B258" s="15"/>
+    </row>
+    <row r="259" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A259" s="18"/>
+      <c r="B259" s="15"/>
+    </row>
+    <row r="260" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A260" s="18"/>
+      <c r="B260" s="15"/>
+    </row>
+    <row r="261" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A261" s="18"/>
+      <c r="B261" s="15"/>
+    </row>
+    <row r="262" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A262" s="18"/>
+      <c r="B262" s="15"/>
+    </row>
+    <row r="263" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A263" s="18"/>
+      <c r="B263" s="15"/>
+    </row>
+    <row r="264" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A264" s="18"/>
+      <c r="B264" s="15"/>
+    </row>
+    <row r="265" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A265" s="18"/>
+      <c r="B265" s="15"/>
+    </row>
+    <row r="266" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A266" s="18"/>
+      <c r="B266" s="15"/>
+    </row>
+    <row r="267" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A267" s="18"/>
+      <c r="B267" s="15"/>
+    </row>
+    <row r="268" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A268" s="18"/>
+      <c r="B268" s="15"/>
+    </row>
+    <row r="269" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A269" s="18"/>
+      <c r="B269" s="15"/>
+    </row>
+    <row r="270" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A270" s="18"/>
+      <c r="B270" s="15"/>
+    </row>
+    <row r="271" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A271" s="18"/>
+      <c r="B271" s="15"/>
+    </row>
+    <row r="272" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A272" s="18"/>
+      <c r="B272" s="15"/>
+    </row>
+    <row r="273" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A273" s="18"/>
+      <c r="B273" s="15"/>
+    </row>
+    <row r="274" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A274" s="18"/>
+      <c r="B274" s="15"/>
+    </row>
+    <row r="275" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A275" s="18"/>
+      <c r="B275" s="15"/>
+    </row>
+    <row r="276" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A276" s="18"/>
+      <c r="B276" s="15"/>
+    </row>
+    <row r="277" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A277" s="18"/>
+      <c r="B277" s="15"/>
+    </row>
+    <row r="278" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A278" s="18"/>
+      <c r="B278" s="15"/>
+    </row>
+    <row r="279" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A279" s="18"/>
+      <c r="B279" s="15"/>
+    </row>
+    <row r="280" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A280" s="18"/>
+      <c r="B280" s="15"/>
+    </row>
+    <row r="281" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A281" s="18"/>
+      <c r="B281" s="15"/>
+    </row>
+    <row r="282" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A282" s="18"/>
+      <c r="B282" s="15"/>
+    </row>
+    <row r="283" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A283" s="18"/>
+      <c r="B283" s="15"/>
+    </row>
+    <row r="284" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A284" s="18"/>
+      <c r="B284" s="15"/>
+    </row>
+    <row r="285" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A285" s="18"/>
+      <c r="B285" s="15"/>
+    </row>
+    <row r="286" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A286" s="18"/>
+      <c r="B286" s="15"/>
+    </row>
+    <row r="287" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A287" s="18"/>
+      <c r="B287" s="15"/>
+    </row>
+    <row r="288" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A288" s="18"/>
+      <c r="B288" s="15"/>
+    </row>
+    <row r="289" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A289" s="18"/>
+      <c r="B289" s="15"/>
+    </row>
+    <row r="290" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A290" s="18"/>
+      <c r="B290" s="15"/>
+    </row>
+    <row r="291" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A291" s="18"/>
+      <c r="B291" s="15"/>
+    </row>
+    <row r="292" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A292" s="18"/>
+      <c r="B292" s="15"/>
+    </row>
+    <row r="293" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A293" s="18"/>
+      <c r="B293" s="15"/>
+    </row>
+    <row r="294" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A294" s="18"/>
+      <c r="B294" s="15"/>
+    </row>
+    <row r="295" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A295" s="18"/>
+      <c r="B295" s="15"/>
+    </row>
+    <row r="296" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A296" s="18"/>
+      <c r="B296" s="15"/>
+    </row>
+    <row r="297" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A297" s="18"/>
+      <c r="B297" s="15"/>
+    </row>
+    <row r="298" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A298" s="18"/>
+      <c r="B298" s="15"/>
+    </row>
+    <row r="299" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A299" s="18"/>
+      <c r="B299" s="15"/>
+    </row>
+    <row r="300" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A300" s="18"/>
+      <c r="B300" s="15"/>
+    </row>
+    <row r="301" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A301" s="18"/>
+      <c r="B301" s="15"/>
+    </row>
+    <row r="302" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A302" s="18"/>
+      <c r="B302" s="15"/>
+    </row>
+    <row r="303" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A303" s="18"/>
+      <c r="B303" s="15"/>
+    </row>
+    <row r="304" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A304" s="18"/>
+      <c r="B304" s="15"/>
+    </row>
+    <row r="305" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A305" s="18"/>
+      <c r="B305" s="15"/>
+    </row>
+    <row r="306" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A306" s="18"/>
+      <c r="B306" s="15"/>
+    </row>
+    <row r="307" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A307" s="18"/>
+      <c r="B307" s="15"/>
+    </row>
+    <row r="308" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A308" s="18"/>
+      <c r="B308" s="15"/>
+    </row>
+    <row r="309" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A309" s="18"/>
+      <c r="B309" s="15"/>
+    </row>
+    <row r="310" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A310" s="18"/>
+      <c r="B310" s="15"/>
+    </row>
+    <row r="311" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A311" s="18"/>
+      <c r="B311" s="15"/>
+    </row>
+    <row r="312" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A312" s="18"/>
+      <c r="B312" s="15"/>
+    </row>
+    <row r="313" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A313" s="18"/>
+      <c r="B313" s="15"/>
+    </row>
+    <row r="314" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A314" s="18"/>
+      <c r="B314" s="15"/>
+    </row>
+    <row r="315" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A315" s="18"/>
+      <c r="B315" s="15"/>
+    </row>
+    <row r="316" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A316" s="18"/>
+      <c r="B316" s="15"/>
+    </row>
+    <row r="317" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A317" s="18"/>
+      <c r="B317" s="15"/>
+    </row>
+    <row r="318" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A318" s="18"/>
+      <c r="B318" s="15"/>
+    </row>
+    <row r="319" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A319" s="18"/>
+      <c r="B319" s="15"/>
+    </row>
+    <row r="320" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A320" s="18"/>
+      <c r="B320" s="15"/>
+    </row>
+    <row r="321" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A321" s="18"/>
+      <c r="B321" s="15"/>
+    </row>
+    <row r="322" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A322" s="18"/>
+      <c r="B322" s="15"/>
+    </row>
+    <row r="323" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A323" s="18"/>
+      <c r="B323" s="15"/>
+    </row>
+    <row r="324" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A324" s="18"/>
+      <c r="B324" s="15"/>
+    </row>
+    <row r="325" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A325" s="18"/>
+      <c r="B325" s="15"/>
+    </row>
+    <row r="326" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A326" s="18"/>
+      <c r="B326" s="15"/>
+    </row>
+    <row r="327" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A327" s="18"/>
+      <c r="B327" s="15"/>
+    </row>
+    <row r="328" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A328" s="18"/>
+      <c r="B328" s="15"/>
+    </row>
+    <row r="329" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A329" s="18"/>
+      <c r="B329" s="15"/>
+    </row>
+    <row r="330" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A330" s="18"/>
+      <c r="B330" s="15"/>
+    </row>
+    <row r="331" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A331" s="18"/>
+      <c r="B331" s="15"/>
+    </row>
+    <row r="332" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A332" s="18"/>
+      <c r="B332" s="15"/>
+    </row>
+    <row r="333" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A333" s="18"/>
+      <c r="B333" s="15"/>
+    </row>
+    <row r="334" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A334" s="18"/>
+      <c r="B334" s="15"/>
+    </row>
+    <row r="335" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A335" s="18"/>
+      <c r="B335" s="15"/>
+    </row>
+    <row r="336" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A336" s="18"/>
+      <c r="B336" s="15"/>
+    </row>
+    <row r="337" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A337" s="18"/>
+      <c r="B337" s="15"/>
+    </row>
+    <row r="338" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A338" s="18"/>
+      <c r="B338" s="15"/>
+    </row>
+    <row r="339" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A339" s="18"/>
+      <c r="B339" s="15"/>
+    </row>
+    <row r="340" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A340" s="18"/>
+      <c r="B340" s="15"/>
+    </row>
+    <row r="341" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A341" s="18"/>
+      <c r="B341" s="15"/>
+    </row>
+    <row r="342" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A342" s="18"/>
+      <c r="B342" s="15"/>
+    </row>
+    <row r="343" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A343" s="18"/>
+      <c r="B343" s="15"/>
+    </row>
+    <row r="344" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A344" s="18"/>
+      <c r="B344" s="15"/>
+    </row>
+    <row r="345" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A345" s="18"/>
+      <c r="B345" s="15"/>
+    </row>
+    <row r="346" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A346" s="18"/>
+      <c r="B346" s="15"/>
+    </row>
+    <row r="347" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A347" s="18"/>
+      <c r="B347" s="15"/>
+    </row>
+    <row r="348" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A348" s="18"/>
+      <c r="B348" s="15"/>
+    </row>
+    <row r="349" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A349" s="18"/>
+      <c r="B349" s="15"/>
+    </row>
+    <row r="350" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A350" s="18"/>
+      <c r="B350" s="15"/>
+    </row>
+    <row r="351" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A351" s="18"/>
+      <c r="B351" s="15"/>
+    </row>
+    <row r="352" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A352" s="18"/>
+      <c r="B352" s="15"/>
+    </row>
+    <row r="353" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A353" s="18"/>
+      <c r="B353" s="15"/>
+    </row>
+    <row r="354" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A354" s="18"/>
+      <c r="B354" s="15"/>
+    </row>
+    <row r="355" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A355" s="18"/>
+      <c r="B355" s="15"/>
+    </row>
+    <row r="356" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A356" s="18"/>
+      <c r="B356" s="15"/>
+    </row>
+    <row r="357" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A357" s="18"/>
+      <c r="B357" s="15"/>
+    </row>
+    <row r="358" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A358" s="18"/>
+      <c r="B358" s="15"/>
+    </row>
+    <row r="359" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A359" s="18"/>
+      <c r="B359" s="15"/>
+    </row>
+    <row r="360" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A360" s="18"/>
+      <c r="B360" s="15"/>
+    </row>
+    <row r="361" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A361" s="18"/>
+      <c r="B361" s="15"/>
+    </row>
+    <row r="362" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A362" s="18"/>
+      <c r="B362" s="15"/>
+    </row>
+    <row r="363" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A363" s="18"/>
+      <c r="B363" s="15"/>
+    </row>
+    <row r="364" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A364" s="18"/>
+      <c r="B364" s="15"/>
+    </row>
+    <row r="365" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A365" s="18"/>
+      <c r="B365" s="15"/>
+    </row>
+    <row r="366" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A366" s="18"/>
+      <c r="B366" s="15"/>
+    </row>
+    <row r="367" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A367" s="18"/>
+      <c r="B367" s="15"/>
+    </row>
+    <row r="368" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A368" s="18"/>
+      <c r="B368" s="15"/>
+    </row>
+    <row r="369" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A369" s="18"/>
+      <c r="B369" s="15"/>
+    </row>
+    <row r="370" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A370" s="18"/>
+      <c r="B370" s="15"/>
+    </row>
+    <row r="371" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A371" s="18"/>
+      <c r="B371" s="15"/>
+    </row>
+    <row r="372" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A372" s="18"/>
+      <c r="B372" s="15"/>
+    </row>
+    <row r="373" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A373" s="18"/>
+      <c r="B373" s="15"/>
+    </row>
+    <row r="374" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A374" s="18"/>
+      <c r="B374" s="15"/>
+    </row>
+    <row r="375" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A375" s="18"/>
+      <c r="B375" s="15"/>
+    </row>
+    <row r="376" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A376" s="18"/>
+      <c r="B376" s="15"/>
+    </row>
+    <row r="377" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A377" s="18"/>
+      <c r="B377" s="15"/>
+    </row>
+    <row r="378" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A378" s="18"/>
+      <c r="B378" s="15"/>
+    </row>
+    <row r="379" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A379" s="18"/>
+      <c r="B379" s="15"/>
+    </row>
+    <row r="380" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A380" s="18"/>
+      <c r="B380" s="15"/>
+    </row>
+    <row r="381" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A381" s="18"/>
+      <c r="B381" s="15"/>
+    </row>
+    <row r="382" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A382" s="18"/>
+      <c r="B382" s="15"/>
+    </row>
+    <row r="383" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A383" s="18"/>
+      <c r="B383" s="15"/>
+    </row>
+    <row r="384" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A384" s="18"/>
+      <c r="B384" s="15"/>
+    </row>
+    <row r="385" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A385" s="18"/>
+      <c r="B385" s="15"/>
+    </row>
+    <row r="386" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A386" s="18"/>
+      <c r="B386" s="15"/>
+    </row>
+    <row r="387" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A387" s="18"/>
+      <c r="B387" s="15"/>
+    </row>
+    <row r="388" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A388" s="18"/>
+      <c r="B388" s="15"/>
+    </row>
+    <row r="389" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A389" s="18"/>
+      <c r="B389" s="15"/>
+    </row>
+    <row r="390" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A390" s="18"/>
+      <c r="B390" s="15"/>
+    </row>
+    <row r="391" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A391" s="18"/>
+      <c r="B391" s="15"/>
+    </row>
+    <row r="392" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A392" s="18"/>
+      <c r="B392" s="15"/>
+    </row>
+    <row r="393" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A393" s="18"/>
+      <c r="B393" s="15"/>
+    </row>
+    <row r="394" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A394" s="18"/>
+      <c r="B394" s="15"/>
+    </row>
+    <row r="395" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A395" s="18"/>
+      <c r="B395" s="15"/>
+    </row>
+    <row r="396" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A396" s="18"/>
+      <c r="B396" s="15"/>
+    </row>
+    <row r="397" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A397" s="18"/>
+      <c r="B397" s="15"/>
+    </row>
+    <row r="398" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A398" s="18"/>
+      <c r="B398" s="15"/>
+    </row>
+    <row r="399" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A399" s="18"/>
+      <c r="B399" s="15"/>
+    </row>
+    <row r="400" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A400" s="18"/>
+      <c r="B400" s="15"/>
+    </row>
+    <row r="401" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A401" s="18"/>
+      <c r="B401" s="15"/>
+    </row>
+    <row r="402" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A402" s="18"/>
+      <c r="B402" s="15"/>
+    </row>
+    <row r="403" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A403" s="18"/>
+      <c r="B403" s="15"/>
+    </row>
+    <row r="404" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A404" s="18"/>
+      <c r="B404" s="15"/>
+    </row>
+    <row r="405" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A405" s="18"/>
+      <c r="B405" s="15"/>
+    </row>
+    <row r="406" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A406" s="18"/>
+      <c r="B406" s="15"/>
+    </row>
+    <row r="407" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A407" s="18"/>
+      <c r="B407" s="15"/>
+    </row>
+    <row r="408" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A408" s="18"/>
+      <c r="B408" s="15"/>
+    </row>
+    <row r="409" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A409" s="18"/>
+      <c r="B409" s="15"/>
+    </row>
+    <row r="410" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A410" s="18"/>
+      <c r="B410" s="15"/>
+    </row>
+    <row r="411" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A411" s="18"/>
+      <c r="B411" s="15"/>
+    </row>
+    <row r="412" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A412" s="18"/>
+      <c r="B412" s="15"/>
+    </row>
+    <row r="413" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A413" s="18"/>
+      <c r="B413" s="15"/>
+    </row>
+    <row r="414" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A414" s="18"/>
+      <c r="B414" s="15"/>
+    </row>
+    <row r="415" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A415" s="18"/>
+      <c r="B415" s="15"/>
+    </row>
+    <row r="416" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A416" s="18"/>
+      <c r="B416" s="15"/>
+    </row>
+    <row r="417" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A417" s="18"/>
+      <c r="B417" s="15"/>
+    </row>
+    <row r="418" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A418" s="18"/>
+      <c r="B418" s="15"/>
+    </row>
+    <row r="419" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A419" s="18"/>
+      <c r="B419" s="15"/>
+    </row>
+    <row r="420" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A420" s="18"/>
+      <c r="B420" s="15"/>
+    </row>
+    <row r="421" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A421" s="18"/>
+      <c r="B421" s="15"/>
+    </row>
+    <row r="422" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A422" s="18"/>
+      <c r="B422" s="15"/>
+    </row>
+    <row r="423" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A423" s="18"/>
+      <c r="B423" s="15"/>
+    </row>
+    <row r="424" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A424" s="18"/>
+      <c r="B424" s="15"/>
+    </row>
+    <row r="425" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A425" s="18"/>
+      <c r="B425" s="15"/>
+    </row>
+    <row r="426" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A426" s="18"/>
+      <c r="B426" s="15"/>
+    </row>
+    <row r="427" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A427" s="18"/>
+      <c r="B427" s="15"/>
+    </row>
+    <row r="428" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A428" s="18"/>
+      <c r="B428" s="15"/>
+    </row>
+    <row r="429" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A429" s="18"/>
+      <c r="B429" s="15"/>
+    </row>
+    <row r="430" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A430" s="18"/>
+      <c r="B430" s="15"/>
+    </row>
+    <row r="431" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A431" s="18"/>
+      <c r="B431" s="15"/>
+    </row>
+    <row r="432" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A432" s="18"/>
+      <c r="B432" s="15"/>
+    </row>
+    <row r="433" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A433" s="18"/>
+      <c r="B433" s="15"/>
+    </row>
+    <row r="434" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A434" s="18"/>
+      <c r="B434" s="15"/>
+    </row>
+    <row r="435" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A435" s="18"/>
+      <c r="B435" s="15"/>
+    </row>
+    <row r="436" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A436" s="18"/>
+      <c r="B436" s="15"/>
+    </row>
+    <row r="437" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A437" s="18"/>
+      <c r="B437" s="15"/>
+    </row>
+    <row r="438" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A438" s="18"/>
+      <c r="B438" s="15"/>
+    </row>
+    <row r="439" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A439" s="18"/>
+      <c r="B439" s="15"/>
+    </row>
+    <row r="440" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A440" s="18"/>
+      <c r="B440" s="15"/>
+    </row>
+    <row r="441" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A441" s="18"/>
+      <c r="B441" s="15"/>
+    </row>
+    <row r="442" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A442" s="18"/>
+      <c r="B442" s="15"/>
+    </row>
+    <row r="443" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A443" s="18"/>
+      <c r="B443" s="15"/>
+    </row>
+    <row r="444" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A444" s="18"/>
+      <c r="B444" s="15"/>
+    </row>
+    <row r="445" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A445" s="18"/>
+      <c r="B445" s="15"/>
+    </row>
+    <row r="446" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A446" s="18"/>
+      <c r="B446" s="15"/>
+    </row>
+    <row r="447" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A447" s="18"/>
+      <c r="B447" s="15"/>
+    </row>
+    <row r="448" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A448" s="18"/>
+      <c r="B448" s="15"/>
+    </row>
+    <row r="449" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A449" s="18"/>
+      <c r="B449" s="15"/>
+    </row>
+    <row r="450" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A450" s="18"/>
+      <c r="B450" s="15"/>
+    </row>
+    <row r="451" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A451" s="18"/>
+      <c r="B451" s="15"/>
+    </row>
+    <row r="452" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A452" s="18"/>
+      <c r="B452" s="15"/>
+    </row>
+    <row r="453" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A453" s="18"/>
+      <c r="B453" s="15"/>
+    </row>
+    <row r="454" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A454" s="18"/>
+      <c r="B454" s="15"/>
+    </row>
+    <row r="455" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A455" s="18"/>
+      <c r="B455" s="15"/>
+    </row>
+    <row r="456" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A456" s="18"/>
+      <c r="B456" s="15"/>
+    </row>
+    <row r="457" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A457" s="18"/>
+      <c r="B457" s="15"/>
+    </row>
+    <row r="458" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A458" s="18"/>
+      <c r="B458" s="15"/>
+    </row>
+    <row r="459" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A459" s="18"/>
+      <c r="B459" s="15"/>
+    </row>
+    <row r="460" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A460" s="18"/>
+      <c r="B460" s="15"/>
+    </row>
+    <row r="461" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A461" s="18"/>
+      <c r="B461" s="15"/>
+    </row>
+    <row r="462" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A462" s="18"/>
+      <c r="B462" s="15"/>
+    </row>
+    <row r="463" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A463" s="18"/>
+      <c r="B463" s="15"/>
+    </row>
+    <row r="464" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A464" s="18"/>
+      <c r="B464" s="15"/>
+    </row>
+    <row r="465" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A465" s="18"/>
+      <c r="B465" s="15"/>
+    </row>
+    <row r="466" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A466" s="18"/>
+      <c r="B466" s="15"/>
+    </row>
+    <row r="467" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A467" s="18"/>
+      <c r="B467" s="15"/>
+    </row>
+    <row r="468" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A468" s="18"/>
+      <c r="B468" s="15"/>
+    </row>
+    <row r="469" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A469" s="18"/>
+      <c r="B469" s="15"/>
+    </row>
+    <row r="470" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A470" s="18"/>
+      <c r="B470" s="15"/>
+    </row>
+    <row r="471" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A471" s="18"/>
+      <c r="B471" s="15"/>
+    </row>
+    <row r="472" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A472" s="18"/>
+      <c r="B472" s="15"/>
+    </row>
+    <row r="473" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A473" s="18"/>
+      <c r="B473" s="15"/>
+    </row>
+    <row r="474" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A474" s="18"/>
+      <c r="B474" s="15"/>
+    </row>
+    <row r="475" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A475" s="18"/>
+      <c r="B475" s="15"/>
+    </row>
+    <row r="476" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A476" s="18"/>
+      <c r="B476" s="15"/>
+    </row>
+    <row r="477" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A477" s="18"/>
+      <c r="B477" s="15"/>
+    </row>
+    <row r="478" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A478" s="18"/>
+      <c r="B478" s="15"/>
+    </row>
+    <row r="479" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A479" s="18"/>
+      <c r="B479" s="15"/>
+    </row>
+    <row r="480" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A480" s="18"/>
+      <c r="B480" s="15"/>
+    </row>
+    <row r="481" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A481" s="18"/>
+      <c r="B481" s="15"/>
+    </row>
+    <row r="482" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A482" s="18"/>
+      <c r="B482" s="15"/>
+    </row>
+    <row r="483" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A483" s="18"/>
+      <c r="B483" s="15"/>
+    </row>
+    <row r="484" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A484" s="18"/>
+      <c r="B484" s="15"/>
+    </row>
+    <row r="485" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A485" s="18"/>
+      <c r="B485" s="15"/>
+    </row>
+    <row r="486" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A486" s="18"/>
+      <c r="B486" s="15"/>
+    </row>
+    <row r="487" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A487" s="18"/>
+      <c r="B487" s="15"/>
+    </row>
+    <row r="488" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A488" s="18"/>
+      <c r="B488" s="15"/>
+    </row>
+    <row r="489" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A489" s="18"/>
+      <c r="B489" s="15"/>
+    </row>
+    <row r="490" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A490" s="18"/>
+      <c r="B490" s="15"/>
+    </row>
+    <row r="491" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A491" s="18"/>
+      <c r="B491" s="15"/>
+    </row>
+    <row r="492" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A492" s="18"/>
+      <c r="B492" s="15"/>
+    </row>
+    <row r="493" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A493" s="18"/>
+      <c r="B493" s="15"/>
+    </row>
+    <row r="494" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A494" s="18"/>
+      <c r="B494" s="15"/>
+    </row>
+    <row r="495" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A495" s="18"/>
+      <c r="B495" s="15"/>
+    </row>
+    <row r="496" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A496" s="18"/>
+      <c r="B496" s="15"/>
+    </row>
+    <row r="497" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A497" s="18"/>
+      <c r="B497" s="15"/>
+    </row>
+    <row r="498" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A498" s="18"/>
+      <c r="B498" s="15"/>
+    </row>
+    <row r="499" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A499" s="18"/>
+      <c r="B499" s="15"/>
+    </row>
+    <row r="500" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A500" s="18"/>
+      <c r="B500" s="15"/>
+    </row>
+    <row r="501" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A501" s="18"/>
+      <c r="B501" s="15"/>
+    </row>
+    <row r="502" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A502" s="18"/>
+      <c r="B502" s="15"/>
+    </row>
+    <row r="503" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A503" s="18"/>
+      <c r="B503" s="15"/>
+    </row>
+    <row r="504" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A504" s="18"/>
+      <c r="B504" s="15"/>
+    </row>
+    <row r="505" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A505" s="18"/>
+      <c r="B505" s="15"/>
+    </row>
+    <row r="506" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A506" s="18"/>
+      <c r="B506" s="15"/>
+    </row>
+    <row r="507" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A507" s="18"/>
+      <c r="B507" s="15"/>
+    </row>
+    <row r="508" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A508" s="18"/>
+      <c r="B508" s="15"/>
+    </row>
+    <row r="509" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A509" s="18"/>
+      <c r="B509" s="15"/>
+    </row>
+    <row r="510" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A510" s="18"/>
+      <c r="B510" s="15"/>
+    </row>
+    <row r="511" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A511" s="18"/>
+      <c r="B511" s="15"/>
+    </row>
+    <row r="512" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A512" s="18"/>
+      <c r="B512" s="15"/>
+    </row>
+    <row r="513" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A513" s="18"/>
+      <c r="B513" s="15"/>
+    </row>
+    <row r="514" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A514" s="18"/>
+      <c r="B514" s="15"/>
+    </row>
+    <row r="515" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A515" s="18"/>
+      <c r="B515" s="15"/>
+    </row>
+    <row r="516" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A516" s="18"/>
+      <c r="B516" s="15"/>
+    </row>
+    <row r="517" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A517" s="18"/>
+      <c r="B517" s="15"/>
+    </row>
+    <row r="518" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A518" s="18"/>
+      <c r="B518" s="15"/>
+    </row>
+    <row r="519" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A519" s="18"/>
+      <c r="B519" s="15"/>
+    </row>
+    <row r="520" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A520" s="18"/>
+      <c r="B520" s="15"/>
+    </row>
+    <row r="521" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A521" s="18"/>
+      <c r="B521" s="15"/>
+    </row>
+    <row r="522" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A522" s="18"/>
+      <c r="B522" s="15"/>
+    </row>
+    <row r="523" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A523" s="18"/>
+      <c r="B523" s="15"/>
+    </row>
+    <row r="524" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A524" s="18"/>
+      <c r="B524" s="15"/>
+    </row>
+    <row r="525" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A525" s="18"/>
+      <c r="B525" s="15"/>
+    </row>
+    <row r="526" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A526" s="18"/>
+      <c r="B526" s="15"/>
+    </row>
+    <row r="527" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A527" s="18"/>
+      <c r="B527" s="15"/>
+    </row>
+    <row r="528" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A528" s="18"/>
+      <c r="B528" s="15"/>
+    </row>
+    <row r="529" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A529" s="18"/>
+      <c r="B529" s="15"/>
+    </row>
+    <row r="530" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A530" s="18"/>
+      <c r="B530" s="15"/>
+    </row>
+    <row r="531" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A531" s="18"/>
+      <c r="B531" s="15"/>
+    </row>
+    <row r="532" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A532" s="18"/>
+      <c r="B532" s="15"/>
+    </row>
+    <row r="533" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A533" s="18"/>
+      <c r="B533" s="15"/>
+    </row>
+    <row r="534" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A534" s="18"/>
+      <c r="B534" s="15"/>
+    </row>
+    <row r="535" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A535" s="18"/>
+      <c r="B535" s="15"/>
+    </row>
+    <row r="536" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A536" s="18"/>
+      <c r="B536" s="15"/>
+    </row>
+    <row r="537" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A537" s="18"/>
+      <c r="B537" s="15"/>
+    </row>
+    <row r="538" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A538" s="18"/>
+      <c r="B538" s="15"/>
+    </row>
+    <row r="539" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A539" s="18"/>
+      <c r="B539" s="15"/>
+    </row>
+    <row r="540" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A540" s="18"/>
+      <c r="B540" s="15"/>
+    </row>
+    <row r="541" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A541" s="18"/>
+      <c r="B541" s="15"/>
+    </row>
+    <row r="542" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A542" s="18"/>
+      <c r="B542" s="15"/>
+    </row>
+    <row r="543" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A543" s="18"/>
+      <c r="B543" s="15"/>
+    </row>
+    <row r="544" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A544" s="18"/>
+      <c r="B544" s="15"/>
+    </row>
+    <row r="545" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A545" s="18"/>
+      <c r="B545" s="15"/>
+    </row>
+    <row r="546" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A546" s="18"/>
+      <c r="B546" s="15"/>
+    </row>
+    <row r="547" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A547" s="18"/>
+      <c r="B547" s="15"/>
+    </row>
+    <row r="548" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A548" s="18"/>
+      <c r="B548" s="15"/>
+    </row>
+    <row r="549" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A549" s="18"/>
+      <c r="B549" s="15"/>
+    </row>
+    <row r="550" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A550" s="18"/>
+      <c r="B550" s="15"/>
+    </row>
+    <row r="551" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A551" s="18"/>
+      <c r="B551" s="15"/>
+    </row>
+    <row r="552" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A552" s="18"/>
+      <c r="B552" s="15"/>
+    </row>
+    <row r="553" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A553" s="18"/>
+      <c r="B553" s="15"/>
+    </row>
+    <row r="554" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A554" s="18"/>
+      <c r="B554" s="15"/>
+    </row>
+    <row r="555" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A555" s="18"/>
+      <c r="B555" s="15"/>
+    </row>
+    <row r="556" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A556" s="18"/>
+      <c r="B556" s="15"/>
+    </row>
+    <row r="557" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A557" s="18"/>
+      <c r="B557" s="15"/>
+    </row>
+    <row r="558" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A558" s="18"/>
+      <c r="B558" s="15"/>
+    </row>
+    <row r="559" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A559" s="18"/>
+      <c r="B559" s="15"/>
+    </row>
+    <row r="560" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A560" s="18"/>
+      <c r="B560" s="15"/>
+    </row>
+    <row r="561" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A561" s="18"/>
+      <c r="B561" s="15"/>
+    </row>
+    <row r="562" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A562" s="18"/>
+      <c r="B562" s="15"/>
+    </row>
+    <row r="563" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A563" s="18"/>
+      <c r="B563" s="15"/>
+    </row>
+    <row r="564" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A564" s="18"/>
+      <c r="B564" s="15"/>
+    </row>
+    <row r="565" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A565" s="18"/>
+      <c r="B565" s="15"/>
+    </row>
+    <row r="566" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A566" s="18"/>
+      <c r="B566" s="15"/>
+    </row>
+    <row r="567" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A567" s="18"/>
+      <c r="B567" s="15"/>
+    </row>
+    <row r="568" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A568" s="18"/>
+      <c r="B568" s="15"/>
+    </row>
+    <row r="569" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A569" s="18"/>
+      <c r="B569" s="15"/>
+    </row>
+    <row r="570" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A570" s="18"/>
+      <c r="B570" s="15"/>
+    </row>
+    <row r="571" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A571" s="18"/>
+      <c r="B571" s="15"/>
+    </row>
+    <row r="572" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A572" s="18"/>
+      <c r="B572" s="15"/>
+    </row>
+    <row r="573" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A573" s="18"/>
+      <c r="B573" s="15"/>
+    </row>
+    <row r="574" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A574" s="18"/>
+      <c r="B574" s="15"/>
+    </row>
+    <row r="575" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A575" s="18"/>
+      <c r="B575" s="15"/>
+    </row>
+    <row r="576" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A576" s="18"/>
+      <c r="B576" s="15"/>
+    </row>
+    <row r="577" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A577" s="18"/>
+      <c r="B577" s="15"/>
+    </row>
+    <row r="578" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A578" s="18"/>
+      <c r="B578" s="15"/>
+    </row>
+    <row r="579" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A579" s="18"/>
+      <c r="B579" s="15"/>
+    </row>
+    <row r="580" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A580" s="18"/>
+      <c r="B580" s="15"/>
+    </row>
+    <row r="581" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A581" s="18"/>
+      <c r="B581" s="15"/>
+    </row>
+    <row r="582" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A582" s="18"/>
+      <c r="B582" s="15"/>
+    </row>
+    <row r="583" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A583" s="18"/>
+      <c r="B583" s="15"/>
+    </row>
+    <row r="584" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A584" s="18"/>
+      <c r="B584" s="15"/>
+    </row>
+    <row r="585" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A585" s="18"/>
+      <c r="B585" s="15"/>
+    </row>
+    <row r="586" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A586" s="18"/>
+      <c r="B586" s="15"/>
+    </row>
+    <row r="587" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A587" s="18"/>
+      <c r="B587" s="15"/>
+    </row>
+    <row r="588" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A588" s="18"/>
+      <c r="B588" s="15"/>
+    </row>
+    <row r="589" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A589" s="18"/>
+      <c r="B589" s="15"/>
+    </row>
+    <row r="590" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A590" s="18"/>
+      <c r="B590" s="15"/>
+    </row>
+    <row r="591" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A591" s="18"/>
+      <c r="B591" s="15"/>
+    </row>
+    <row r="592" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A592" s="18"/>
+      <c r="B592" s="15"/>
+    </row>
+    <row r="593" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A593" s="18"/>
+      <c r="B593" s="15"/>
+    </row>
+    <row r="594" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A594" s="18"/>
+      <c r="B594" s="15"/>
+    </row>
+    <row r="595" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A595" s="18"/>
+      <c r="B595" s="15"/>
+    </row>
+    <row r="596" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A596" s="18"/>
+      <c r="B596" s="15"/>
+    </row>
+    <row r="597" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A597" s="18"/>
+      <c r="B597" s="15"/>
+    </row>
+    <row r="598" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A598" s="18"/>
+      <c r="B598" s="15"/>
+    </row>
+    <row r="599" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A599" s="18"/>
+      <c r="B599" s="15"/>
+    </row>
+    <row r="600" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A600" s="18"/>
+      <c r="B600" s="15"/>
+    </row>
+    <row r="601" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A601" s="18"/>
+      <c r="B601" s="15"/>
+    </row>
+    <row r="602" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A602" s="18"/>
+      <c r="B602" s="15"/>
+    </row>
+    <row r="603" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A603" s="18"/>
+      <c r="B603" s="15"/>
+    </row>
+    <row r="604" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A604" s="18"/>
+      <c r="B604" s="15"/>
+    </row>
+    <row r="605" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A605" s="18"/>
+      <c r="B605" s="15"/>
+    </row>
+    <row r="606" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A606" s="18"/>
+      <c r="B606" s="15"/>
+    </row>
+    <row r="607" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A607" s="18"/>
+      <c r="B607" s="15"/>
+    </row>
+    <row r="608" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A608" s="18"/>
+      <c r="B608" s="15"/>
+    </row>
+    <row r="609" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A609" s="18"/>
+      <c r="B609" s="15"/>
+    </row>
+    <row r="610" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A610" s="18"/>
+      <c r="B610" s="15"/>
+    </row>
+    <row r="611" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A611" s="18"/>
+      <c r="B611" s="15"/>
+    </row>
+    <row r="612" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A612" s="18"/>
+      <c r="B612" s="15"/>
+    </row>
+    <row r="613" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A613" s="18"/>
+      <c r="B613" s="15"/>
+    </row>
+    <row r="614" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A614" s="18"/>
+      <c r="B614" s="15"/>
+    </row>
+    <row r="615" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A615" s="18"/>
+      <c r="B615" s="15"/>
+    </row>
+    <row r="616" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A616" s="18"/>
+      <c r="B616" s="15"/>
+    </row>
+    <row r="617" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A617" s="18"/>
+      <c r="B617" s="15"/>
+    </row>
+    <row r="618" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A618" s="18"/>
+      <c r="B618" s="15"/>
+    </row>
+    <row r="619" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A619" s="18"/>
+      <c r="B619" s="15"/>
+    </row>
+    <row r="620" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A620" s="18"/>
+      <c r="B620" s="15"/>
+    </row>
+    <row r="621" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A621" s="18"/>
+      <c r="B621" s="15"/>
+    </row>
+    <row r="622" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A622" s="18"/>
+      <c r="B622" s="15"/>
+    </row>
+    <row r="623" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A623" s="18"/>
+      <c r="B623" s="15"/>
+    </row>
+    <row r="624" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A624" s="18"/>
+      <c r="B624" s="15"/>
+    </row>
+    <row r="625" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A625" s="18"/>
+      <c r="B625" s="15"/>
+    </row>
+    <row r="626" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A626" s="18"/>
+      <c r="B626" s="15"/>
+    </row>
+    <row r="627" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A627" s="18"/>
+      <c r="B627" s="15"/>
+    </row>
+    <row r="628" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A628" s="18"/>
+      <c r="B628" s="15"/>
+    </row>
+    <row r="629" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A629" s="18"/>
+      <c r="B629" s="15"/>
+    </row>
+    <row r="630" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A630" s="18"/>
+      <c r="B630" s="15"/>
+    </row>
+    <row r="631" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A631" s="18"/>
+      <c r="B631" s="15"/>
+    </row>
+    <row r="632" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A632" s="18"/>
+      <c r="B632" s="15"/>
+    </row>
+    <row r="633" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A633" s="18"/>
+      <c r="B633" s="15"/>
+    </row>
+    <row r="634" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A634" s="18"/>
+      <c r="B634" s="15"/>
+    </row>
+    <row r="635" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A635" s="18"/>
+      <c r="B635" s="15"/>
+    </row>
+    <row r="636" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A636" s="18"/>
+      <c r="B636" s="15"/>
+    </row>
+    <row r="637" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A637" s="18"/>
+      <c r="B637" s="15"/>
+    </row>
+    <row r="638" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A638" s="18"/>
+      <c r="B638" s="15"/>
+    </row>
+    <row r="639" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A639" s="18"/>
+      <c r="B639" s="15"/>
+    </row>
+    <row r="640" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A640" s="18"/>
+      <c r="B640" s="15"/>
+    </row>
+    <row r="641" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A641" s="18"/>
+      <c r="B641" s="15"/>
+    </row>
+    <row r="642" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A642" s="18"/>
+      <c r="B642" s="15"/>
+    </row>
+    <row r="643" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A643" s="18"/>
+      <c r="B643" s="15"/>
+    </row>
+    <row r="644" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A644" s="18"/>
+      <c r="B644" s="15"/>
+    </row>
+    <row r="645" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A645" s="18"/>
+      <c r="B645" s="15"/>
+    </row>
+    <row r="646" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A646" s="18"/>
+      <c r="B646" s="15"/>
+    </row>
+    <row r="647" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A647" s="18"/>
+      <c r="B647" s="15"/>
+    </row>
+    <row r="648" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A648" s="18"/>
+      <c r="B648" s="15"/>
+    </row>
+    <row r="649" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A649" s="18"/>
+      <c r="B649" s="15"/>
+    </row>
+    <row r="650" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A650" s="18"/>
+      <c r="B650" s="15"/>
+    </row>
+    <row r="651" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A651" s="18"/>
+      <c r="B651" s="15"/>
+    </row>
+    <row r="652" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A652" s="18"/>
+      <c r="B652" s="15"/>
+    </row>
+    <row r="653" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A653" s="18"/>
+      <c r="B653" s="15"/>
+    </row>
+    <row r="654" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A654" s="18"/>
+      <c r="B654" s="15"/>
+    </row>
+    <row r="655" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A655" s="18"/>
+      <c r="B655" s="15"/>
+    </row>
+    <row r="656" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A656" s="18"/>
+      <c r="B656" s="15"/>
+    </row>
+    <row r="657" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A657" s="18"/>
+      <c r="B657" s="15"/>
+    </row>
+    <row r="658" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A658" s="18"/>
+      <c r="B658" s="15"/>
+    </row>
+    <row r="659" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A659" s="18"/>
+      <c r="B659" s="15"/>
+    </row>
+    <row r="660" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A660" s="18"/>
+      <c r="B660" s="15"/>
+    </row>
+    <row r="661" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A661" s="18"/>
+      <c r="B661" s="15"/>
+    </row>
+    <row r="662" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A662" s="18"/>
+      <c r="B662" s="15"/>
+    </row>
+    <row r="663" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A663" s="18"/>
+      <c r="B663" s="15"/>
+    </row>
+    <row r="664" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A664" s="18"/>
+      <c r="B664" s="15"/>
+    </row>
+    <row r="665" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A665" s="18"/>
+      <c r="B665" s="15"/>
+    </row>
+    <row r="666" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A666" s="18"/>
+      <c r="B666" s="15"/>
+    </row>
+    <row r="667" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A667" s="18"/>
+      <c r="B667" s="15"/>
+    </row>
+    <row r="668" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A668" s="18"/>
+      <c r="B668" s="15"/>
+    </row>
+    <row r="669" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A669" s="18"/>
+      <c r="B669" s="15"/>
+    </row>
+    <row r="670" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A670" s="18"/>
+      <c r="B670" s="15"/>
+    </row>
+    <row r="671" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A671" s="18"/>
+      <c r="B671" s="15"/>
+    </row>
+    <row r="672" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A672" s="18"/>
+      <c r="B672" s="15"/>
+    </row>
+    <row r="673" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A673" s="18"/>
+      <c r="B673" s="15"/>
+    </row>
+    <row r="674" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A674" s="18"/>
+      <c r="B674" s="15"/>
+    </row>
+    <row r="675" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A675" s="18"/>
+      <c r="B675" s="15"/>
+    </row>
+    <row r="676" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A676" s="18"/>
+      <c r="B676" s="15"/>
+    </row>
+    <row r="677" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A677" s="18"/>
+      <c r="B677" s="15"/>
+    </row>
+    <row r="678" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A678" s="18"/>
+      <c r="B678" s="15"/>
+    </row>
+    <row r="679" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A679" s="18"/>
+      <c r="B679" s="15"/>
+    </row>
+    <row r="680" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A680" s="18"/>
+      <c r="B680" s="15"/>
+    </row>
+    <row r="681" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A681" s="18"/>
+      <c r="B681" s="15"/>
+    </row>
+    <row r="682" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A682" s="18"/>
+      <c r="B682" s="15"/>
+    </row>
+    <row r="683" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A683" s="18"/>
+      <c r="B683" s="15"/>
+    </row>
+    <row r="684" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A684" s="18"/>
+      <c r="B684" s="15"/>
+    </row>
+    <row r="685" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A685" s="18"/>
+      <c r="B685" s="15"/>
+    </row>
+    <row r="686" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A686" s="18"/>
+      <c r="B686" s="15"/>
+    </row>
+    <row r="687" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A687" s="18"/>
+      <c r="B687" s="15"/>
+    </row>
+    <row r="688" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A688" s="18"/>
+      <c r="B688" s="15"/>
+    </row>
+    <row r="689" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A689" s="18"/>
+      <c r="B689" s="15"/>
+    </row>
+    <row r="690" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A690" s="18"/>
+      <c r="B690" s="15"/>
+    </row>
+    <row r="691" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A691" s="18"/>
+      <c r="B691" s="15"/>
+    </row>
+    <row r="692" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A692" s="18"/>
+      <c r="B692" s="15"/>
+    </row>
+    <row r="693" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A693" s="18"/>
+      <c r="B693" s="15"/>
+    </row>
+    <row r="694" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A694" s="18"/>
+      <c r="B694" s="15"/>
+    </row>
+    <row r="695" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A695" s="18"/>
+      <c r="B695" s="15"/>
+    </row>
+    <row r="696" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A696" s="18"/>
+      <c r="B696" s="15"/>
+    </row>
+    <row r="697" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A697" s="18"/>
+      <c r="B697" s="15"/>
+    </row>
+    <row r="698" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A698" s="18"/>
+      <c r="B698" s="15"/>
+    </row>
+    <row r="699" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A699" s="18"/>
+      <c r="B699" s="15"/>
+    </row>
+    <row r="700" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A700" s="18"/>
+      <c r="B700" s="15"/>
+    </row>
+    <row r="701" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A701" s="18"/>
+      <c r="B701" s="15"/>
+    </row>
+    <row r="702" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A702" s="18"/>
+      <c r="B702" s="15"/>
+    </row>
+    <row r="703" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A703" s="18"/>
+      <c r="B703" s="15"/>
+    </row>
+    <row r="704" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A704" s="18"/>
+      <c r="B704" s="15"/>
+    </row>
+    <row r="705" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A705" s="18"/>
+      <c r="B705" s="15"/>
+    </row>
+    <row r="706" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A706" s="18"/>
+      <c r="B706" s="15"/>
+    </row>
+    <row r="707" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A707" s="18"/>
+      <c r="B707" s="15"/>
+    </row>
+    <row r="708" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A708" s="18"/>
+      <c r="B708" s="15"/>
+    </row>
+    <row r="709" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A709" s="18"/>
+      <c r="B709" s="15"/>
+    </row>
+    <row r="710" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A710" s="18"/>
+      <c r="B710" s="15"/>
+    </row>
+    <row r="711" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A711" s="18"/>
+      <c r="B711" s="15"/>
+    </row>
+    <row r="712" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A712" s="18"/>
+      <c r="B712" s="15"/>
+    </row>
+    <row r="713" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A713" s="18"/>
+      <c r="B713" s="15"/>
+    </row>
+    <row r="714" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A714" s="18"/>
+      <c r="B714" s="15"/>
+    </row>
+    <row r="715" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A715" s="18"/>
+      <c r="B715" s="15"/>
+    </row>
+    <row r="716" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A716" s="18"/>
+      <c r="B716" s="15"/>
+    </row>
+    <row r="717" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A717" s="18"/>
+      <c r="B717" s="15"/>
+    </row>
+    <row r="718" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A718" s="18"/>
+      <c r="B718" s="15"/>
+    </row>
+    <row r="719" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A719" s="18"/>
+      <c r="B719" s="15"/>
+    </row>
+    <row r="720" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A720" s="18"/>
+      <c r="B720" s="15"/>
+    </row>
+    <row r="721" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A721" s="18"/>
+      <c r="B721" s="15"/>
+    </row>
+    <row r="722" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A722" s="18"/>
+      <c r="B722" s="15"/>
+    </row>
+    <row r="723" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A723" s="18"/>
+      <c r="B723" s="15"/>
+    </row>
+    <row r="724" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A724" s="18"/>
+      <c r="B724" s="15"/>
+    </row>
+    <row r="725" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A725" s="18"/>
+      <c r="B725" s="15"/>
+    </row>
+    <row r="726" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A726" s="18"/>
+      <c r="B726" s="15"/>
+    </row>
+    <row r="727" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A727" s="18"/>
+      <c r="B727" s="15"/>
+    </row>
+    <row r="728" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A728" s="18"/>
+      <c r="B728" s="15"/>
+    </row>
+    <row r="729" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A729" s="18"/>
+      <c r="B729" s="15"/>
+    </row>
+    <row r="730" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A730" s="18"/>
+      <c r="B730" s="15"/>
+    </row>
+    <row r="731" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A731" s="18"/>
+      <c r="B731" s="15"/>
+    </row>
+    <row r="732" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A732" s="18"/>
+      <c r="B732" s="15"/>
+    </row>
+    <row r="733" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A733" s="18"/>
+      <c r="B733" s="15"/>
+    </row>
+    <row r="734" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A734" s="18"/>
+      <c r="B734" s="15"/>
+    </row>
+    <row r="735" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A735" s="18"/>
+      <c r="B735" s="15"/>
+    </row>
+    <row r="736" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A736" s="18"/>
+      <c r="B736" s="15"/>
+    </row>
+    <row r="737" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A737" s="18"/>
+      <c r="B737" s="15"/>
+    </row>
+    <row r="738" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A738" s="18"/>
+      <c r="B738" s="15"/>
+    </row>
+    <row r="739" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A739" s="18"/>
+      <c r="B739" s="15"/>
+    </row>
+    <row r="740" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A740" s="18"/>
+      <c r="B740" s="15"/>
+    </row>
+    <row r="741" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A741" s="18"/>
+      <c r="B741" s="15"/>
+    </row>
+    <row r="742" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A742" s="18"/>
+      <c r="B742" s="15"/>
+    </row>
+    <row r="743" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A743" s="18"/>
+      <c r="B743" s="15"/>
+    </row>
+    <row r="744" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A744" s="18"/>
+      <c r="B744" s="15"/>
+    </row>
+    <row r="745" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A745" s="18"/>
+      <c r="B745" s="15"/>
+    </row>
+    <row r="746" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A746" s="18"/>
+      <c r="B746" s="15"/>
+    </row>
+    <row r="747" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A747" s="18"/>
+      <c r="B747" s="15"/>
+    </row>
+    <row r="748" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A748" s="18"/>
+      <c r="B748" s="15"/>
+    </row>
+    <row r="749" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A749" s="18"/>
+      <c r="B749" s="15"/>
+    </row>
+    <row r="750" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A750" s="18"/>
+      <c r="B750" s="15"/>
+    </row>
+    <row r="751" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A751" s="18"/>
+      <c r="B751" s="15"/>
+    </row>
+    <row r="752" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A752" s="18"/>
+      <c r="B752" s="15"/>
+    </row>
+    <row r="753" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A753" s="18"/>
+      <c r="B753" s="15"/>
+    </row>
+    <row r="754" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A754" s="18"/>
+      <c r="B754" s="15"/>
+    </row>
+    <row r="755" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A755" s="18"/>
+      <c r="B755" s="15"/>
+    </row>
+    <row r="756" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A756" s="18"/>
+      <c r="B756" s="15"/>
+    </row>
+    <row r="757" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A757" s="18"/>
+      <c r="B757" s="15"/>
+    </row>
+    <row r="758" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A758" s="18"/>
+      <c r="B758" s="15"/>
+    </row>
+    <row r="759" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A759" s="18"/>
+      <c r="B759" s="15"/>
+    </row>
+    <row r="760" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A760" s="18"/>
+      <c r="B760" s="15"/>
+    </row>
+    <row r="761" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A761" s="18"/>
+      <c r="B761" s="15"/>
+    </row>
+    <row r="762" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A762" s="18"/>
+      <c r="B762" s="15"/>
+    </row>
+    <row r="763" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A763" s="18"/>
+      <c r="B763" s="15"/>
+    </row>
+    <row r="764" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A764" s="18"/>
+      <c r="B764" s="15"/>
+    </row>
+    <row r="765" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A765" s="18"/>
+      <c r="B765" s="15"/>
+    </row>
+    <row r="766" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A766" s="18"/>
+      <c r="B766" s="15"/>
+    </row>
+    <row r="767" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A767" s="18"/>
+      <c r="B767" s="15"/>
+    </row>
+    <row r="768" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A768" s="18"/>
+      <c r="B768" s="15"/>
+    </row>
+    <row r="769" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A769" s="18"/>
+      <c r="B769" s="15"/>
+    </row>
+    <row r="770" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A770" s="18"/>
+      <c r="B770" s="15"/>
+    </row>
+    <row r="771" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A771" s="18"/>
+      <c r="B771" s="15"/>
+    </row>
+    <row r="772" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A772" s="18"/>
+      <c r="B772" s="15"/>
+    </row>
+    <row r="773" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A773" s="18"/>
+      <c r="B773" s="15"/>
+    </row>
+    <row r="774" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A774" s="18"/>
+      <c r="B774" s="15"/>
+    </row>
+    <row r="775" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A775" s="18"/>
+      <c r="B775" s="15"/>
+    </row>
+    <row r="776" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A776" s="18"/>
+      <c r="B776" s="15"/>
+    </row>
+    <row r="777" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A777" s="18"/>
+      <c r="B777" s="15"/>
+    </row>
+    <row r="778" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A778" s="18"/>
+      <c r="B778" s="15"/>
+    </row>
+    <row r="779" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A779" s="18"/>
+      <c r="B779" s="15"/>
+    </row>
+    <row r="780" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A780" s="18"/>
+      <c r="B780" s="15"/>
+    </row>
+    <row r="781" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A781" s="18"/>
+      <c r="B781" s="15"/>
+    </row>
+    <row r="782" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A782" s="18"/>
+      <c r="B782" s="15"/>
+    </row>
+    <row r="783" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A783" s="18"/>
+      <c r="B783" s="15"/>
+    </row>
+    <row r="784" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A784" s="18"/>
+      <c r="B784" s="15"/>
+    </row>
+    <row r="785" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A785" s="18"/>
+      <c r="B785" s="15"/>
+    </row>
+    <row r="786" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A786" s="18"/>
+      <c r="B786" s="15"/>
+    </row>
+    <row r="787" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A787" s="18"/>
+      <c r="B787" s="15"/>
+    </row>
+    <row r="788" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A788" s="18"/>
+      <c r="B788" s="15"/>
+    </row>
+    <row r="789" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A789" s="18"/>
+      <c r="B789" s="15"/>
+    </row>
+    <row r="790" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A790" s="18"/>
+      <c r="B790" s="15"/>
+    </row>
+    <row r="791" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A791" s="18"/>
+      <c r="B791" s="15"/>
+    </row>
+    <row r="792" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A792" s="18"/>
+      <c r="B792" s="15"/>
+    </row>
+    <row r="793" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A793" s="18"/>
+      <c r="B793" s="15"/>
+    </row>
+    <row r="794" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A794" s="18"/>
+      <c r="B794" s="15"/>
+    </row>
+    <row r="795" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A795" s="18"/>
+      <c r="B795" s="15"/>
+    </row>
+    <row r="796" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A796" s="18"/>
+      <c r="B796" s="15"/>
+    </row>
+    <row r="797" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A797" s="18"/>
+      <c r="B797" s="15"/>
+    </row>
+    <row r="798" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A798" s="18"/>
+      <c r="B798" s="15"/>
+    </row>
+    <row r="799" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A799" s="18"/>
+      <c r="B799" s="15"/>
+    </row>
+    <row r="800" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A800" s="18"/>
+      <c r="B800" s="15"/>
+    </row>
+    <row r="801" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A801" s="18"/>
+      <c r="B801" s="15"/>
+    </row>
+    <row r="802" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A802" s="18"/>
+      <c r="B802" s="15"/>
+    </row>
+    <row r="803" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A803" s="18"/>
+      <c r="B803" s="15"/>
+    </row>
+    <row r="804" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A804" s="18"/>
+      <c r="B804" s="15"/>
+    </row>
+    <row r="805" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A805" s="18"/>
+      <c r="B805" s="15"/>
+    </row>
+    <row r="806" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A806" s="18"/>
+      <c r="B806" s="15"/>
+    </row>
+    <row r="807" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A807" s="18"/>
+      <c r="B807" s="15"/>
+    </row>
+    <row r="808" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A808" s="18"/>
+      <c r="B808" s="15"/>
+    </row>
+    <row r="809" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A809" s="18"/>
+      <c r="B809" s="15"/>
+    </row>
+    <row r="810" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A810" s="18"/>
+      <c r="B810" s="15"/>
+    </row>
+    <row r="811" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A811" s="18"/>
+      <c r="B811" s="15"/>
+    </row>
+    <row r="812" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A812" s="18"/>
+      <c r="B812" s="15"/>
+    </row>
+    <row r="813" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A813" s="18"/>
+      <c r="B813" s="15"/>
+    </row>
+    <row r="814" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A814" s="18"/>
+      <c r="B814" s="15"/>
+    </row>
+    <row r="815" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A815" s="18"/>
+      <c r="B815" s="15"/>
+    </row>
+    <row r="816" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A816" s="18"/>
+      <c r="B816" s="15"/>
+    </row>
+    <row r="817" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A817" s="18"/>
+      <c r="B817" s="15"/>
+    </row>
+    <row r="818" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A818" s="18"/>
+      <c r="B818" s="15"/>
+    </row>
+    <row r="819" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A819" s="18"/>
+      <c r="B819" s="15"/>
+    </row>
+    <row r="820" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A820" s="18"/>
+      <c r="B820" s="15"/>
+    </row>
+    <row r="821" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A821" s="18"/>
+      <c r="B821" s="15"/>
+    </row>
+    <row r="822" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A822" s="18"/>
+      <c r="B822" s="15"/>
+    </row>
+    <row r="823" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A823" s="18"/>
+      <c r="B823" s="15"/>
+    </row>
+    <row r="824" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A824" s="18"/>
+      <c r="B824" s="15"/>
+    </row>
+    <row r="825" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A825" s="18"/>
+      <c r="B825" s="15"/>
+    </row>
+    <row r="826" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A826" s="18"/>
+      <c r="B826" s="15"/>
+    </row>
+    <row r="827" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A827" s="18"/>
+      <c r="B827" s="15"/>
+    </row>
+    <row r="828" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A828" s="18"/>
+      <c r="B828" s="15"/>
+    </row>
+    <row r="829" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A829" s="18"/>
+      <c r="B829" s="15"/>
+    </row>
+    <row r="830" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A830" s="18"/>
+      <c r="B830" s="15"/>
+    </row>
+    <row r="831" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A831" s="18"/>
+      <c r="B831" s="15"/>
+    </row>
+    <row r="832" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A832" s="18"/>
+      <c r="B832" s="15"/>
+    </row>
+    <row r="833" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A833" s="18"/>
+      <c r="B833" s="15"/>
+    </row>
+    <row r="834" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A834" s="18"/>
+      <c r="B834" s="15"/>
+    </row>
+    <row r="835" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A835" s="18"/>
+      <c r="B835" s="15"/>
+    </row>
+    <row r="836" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A836" s="18"/>
+      <c r="B836" s="15"/>
+    </row>
+    <row r="837" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A837" s="18"/>
+      <c r="B837" s="15"/>
+    </row>
+    <row r="838" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A838" s="18"/>
+      <c r="B838" s="15"/>
+    </row>
+    <row r="839" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A839" s="18"/>
+      <c r="B839" s="15"/>
+    </row>
+    <row r="840" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A840" s="18"/>
+      <c r="B840" s="15"/>
+    </row>
+    <row r="841" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A841" s="18"/>
+      <c r="B841" s="15"/>
+    </row>
+    <row r="842" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A842" s="18"/>
+      <c r="B842" s="15"/>
+    </row>
+    <row r="843" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A843" s="18"/>
+      <c r="B843" s="15"/>
+    </row>
+    <row r="844" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A844" s="18"/>
+      <c r="B844" s="15"/>
+    </row>
+    <row r="845" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A845" s="18"/>
+      <c r="B845" s="15"/>
+    </row>
+    <row r="846" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A846" s="18"/>
+      <c r="B846" s="15"/>
+    </row>
+    <row r="847" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A847" s="18"/>
+      <c r="B847" s="15"/>
+    </row>
+    <row r="848" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A848" s="18"/>
+      <c r="B848" s="15"/>
+    </row>
+    <row r="849" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A849" s="18"/>
+      <c r="B849" s="15"/>
+    </row>
+    <row r="850" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A850" s="18"/>
+      <c r="B850" s="15"/>
+    </row>
+    <row r="851" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A851" s="18"/>
+      <c r="B851" s="15"/>
+    </row>
+    <row r="852" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A852" s="18"/>
+      <c r="B852" s="15"/>
+    </row>
+    <row r="853" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A853" s="18"/>
+      <c r="B853" s="15"/>
+    </row>
+    <row r="854" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A854" s="18"/>
+      <c r="B854" s="15"/>
+    </row>
+    <row r="855" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A855" s="18"/>
+      <c r="B855" s="15"/>
+    </row>
+    <row r="856" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A856" s="18"/>
+      <c r="B856" s="15"/>
+    </row>
+    <row r="857" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A857" s="18"/>
+      <c r="B857" s="15"/>
+    </row>
+    <row r="858" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A858" s="18"/>
+      <c r="B858" s="15"/>
+    </row>
+    <row r="859" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A859" s="18"/>
+      <c r="B859" s="15"/>
+    </row>
+    <row r="860" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A860" s="18"/>
+      <c r="B860" s="15"/>
+    </row>
+    <row r="861" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A861" s="18"/>
+      <c r="B861" s="15"/>
+    </row>
+    <row r="862" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A862" s="18"/>
+      <c r="B862" s="15"/>
+    </row>
+    <row r="863" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A863" s="18"/>
+      <c r="B863" s="15"/>
+    </row>
+    <row r="864" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A864" s="18"/>
+      <c r="B864" s="15"/>
+    </row>
+    <row r="865" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A865" s="18"/>
+      <c r="B865" s="15"/>
+    </row>
+    <row r="866" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A866" s="18"/>
+      <c r="B866" s="15"/>
+    </row>
+    <row r="867" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A867" s="18"/>
+      <c r="B867" s="15"/>
+    </row>
+    <row r="868" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A868" s="18"/>
+      <c r="B868" s="15"/>
+    </row>
+    <row r="869" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A869" s="18"/>
+      <c r="B869" s="15"/>
+    </row>
+    <row r="870" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A870" s="18"/>
+      <c r="B870" s="15"/>
+    </row>
+    <row r="871" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A871" s="18"/>
+      <c r="B871" s="15"/>
+    </row>
+    <row r="872" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A872" s="18"/>
+      <c r="B872" s="15"/>
+    </row>
+    <row r="873" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A873" s="18"/>
+      <c r="B873" s="15"/>
+    </row>
+    <row r="874" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A874" s="18"/>
+      <c r="B874" s="15"/>
+    </row>
+    <row r="875" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A875" s="18"/>
+      <c r="B875" s="15"/>
+    </row>
+    <row r="876" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A876" s="18"/>
+      <c r="B876" s="15"/>
+    </row>
+    <row r="877" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A877" s="18"/>
+      <c r="B877" s="15"/>
+    </row>
+    <row r="878" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A878" s="18"/>
+      <c r="B878" s="15"/>
+    </row>
+    <row r="879" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A879" s="18"/>
+      <c r="B879" s="15"/>
+    </row>
+    <row r="880" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A880" s="18"/>
+      <c r="B880" s="15"/>
+    </row>
+    <row r="881" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A881" s="18"/>
+      <c r="B881" s="15"/>
+    </row>
+    <row r="882" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A882" s="18"/>
+      <c r="B882" s="15"/>
+    </row>
+    <row r="883" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A883" s="18"/>
+      <c r="B883" s="15"/>
+    </row>
+    <row r="884" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A884" s="18"/>
+      <c r="B884" s="15"/>
+    </row>
+    <row r="885" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A885" s="18"/>
+      <c r="B885" s="15"/>
+    </row>
+    <row r="886" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A886" s="18"/>
+      <c r="B886" s="15"/>
+    </row>
+    <row r="887" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A887" s="18"/>
+      <c r="B887" s="15"/>
+    </row>
+    <row r="888" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A888" s="18"/>
+      <c r="B888" s="15"/>
+    </row>
+    <row r="889" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A889" s="18"/>
+      <c r="B889" s="15"/>
+    </row>
+    <row r="890" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A890" s="18"/>
+      <c r="B890" s="15"/>
+    </row>
+    <row r="891" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A891" s="18"/>
+      <c r="B891" s="15"/>
+    </row>
+    <row r="892" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A892" s="18"/>
+      <c r="B892" s="15"/>
+    </row>
+    <row r="893" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A893" s="18"/>
+      <c r="B893" s="15"/>
+    </row>
+    <row r="894" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A894" s="18"/>
+      <c r="B894" s="15"/>
+    </row>
+    <row r="895" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A895" s="18"/>
+      <c r="B895" s="15"/>
+    </row>
+    <row r="896" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A896" s="18"/>
+      <c r="B896" s="15"/>
+    </row>
+    <row r="897" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A897" s="18"/>
+      <c r="B897" s="15"/>
+    </row>
+    <row r="898" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A898" s="18"/>
+      <c r="B898" s="15"/>
+    </row>
+    <row r="899" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A899" s="18"/>
+      <c r="B899" s="15"/>
+    </row>
+    <row r="900" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A900" s="18"/>
+      <c r="B900" s="15"/>
+    </row>
+    <row r="901" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A901" s="18"/>
+      <c r="B901" s="15"/>
+    </row>
+    <row r="902" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A902" s="18"/>
+      <c r="B902" s="15"/>
+    </row>
+    <row r="903" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A903" s="18"/>
+      <c r="B903" s="15"/>
+    </row>
+    <row r="904" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A904" s="18"/>
+      <c r="B904" s="15"/>
+    </row>
+    <row r="905" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A905" s="18"/>
+      <c r="B905" s="15"/>
+    </row>
+    <row r="906" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A906" s="18"/>
+      <c r="B906" s="15"/>
+    </row>
+    <row r="907" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A907" s="18"/>
+      <c r="B907" s="15"/>
+    </row>
+    <row r="908" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A908" s="18"/>
+      <c r="B908" s="15"/>
+    </row>
+    <row r="909" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A909" s="18"/>
+      <c r="B909" s="15"/>
+    </row>
+    <row r="910" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A910" s="18"/>
+      <c r="B910" s="15"/>
+    </row>
+    <row r="911" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A911" s="18"/>
+      <c r="B911" s="15"/>
+    </row>
+    <row r="912" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A912" s="18"/>
+      <c r="B912" s="15"/>
+    </row>
+    <row r="913" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A913" s="18"/>
+      <c r="B913" s="15"/>
+    </row>
+    <row r="914" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A914" s="18"/>
+      <c r="B914" s="15"/>
+    </row>
+    <row r="915" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A915" s="18"/>
+      <c r="B915" s="15"/>
+    </row>
+    <row r="916" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A916" s="18"/>
+      <c r="B916" s="15"/>
+    </row>
+    <row r="917" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A917" s="18"/>
+      <c r="B917" s="15"/>
+    </row>
+    <row r="918" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A918" s="18"/>
+      <c r="B918" s="15"/>
+    </row>
+    <row r="919" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A919" s="18"/>
+      <c r="B919" s="15"/>
+    </row>
+    <row r="920" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A920" s="18"/>
+      <c r="B920" s="15"/>
+    </row>
+    <row r="921" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A921" s="18"/>
+      <c r="B921" s="15"/>
+    </row>
+    <row r="922" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A922" s="18"/>
+      <c r="B922" s="15"/>
+    </row>
+    <row r="923" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A923" s="18"/>
+      <c r="B923" s="15"/>
+    </row>
+    <row r="924" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A924" s="18"/>
+      <c r="B924" s="15"/>
+    </row>
+    <row r="925" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A925" s="18"/>
+      <c r="B925" s="15"/>
+    </row>
+    <row r="926" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A926" s="18"/>
+      <c r="B926" s="15"/>
+    </row>
+    <row r="927" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A927" s="18"/>
+      <c r="B927" s="15"/>
+    </row>
+    <row r="928" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A928" s="18"/>
+      <c r="B928" s="15"/>
+    </row>
+    <row r="929" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A929" s="18"/>
+      <c r="B929" s="15"/>
+    </row>
+    <row r="930" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A930" s="18"/>
+      <c r="B930" s="15"/>
+    </row>
+    <row r="931" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A931" s="18"/>
+      <c r="B931" s="15"/>
+    </row>
+    <row r="932" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A932" s="18"/>
+      <c r="B932" s="15"/>
+    </row>
+    <row r="933" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A933" s="18"/>
+      <c r="B933" s="15"/>
+    </row>
+    <row r="934" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A934" s="18"/>
+      <c r="B934" s="15"/>
+    </row>
+    <row r="935" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A935" s="18"/>
+      <c r="B935" s="15"/>
+    </row>
+    <row r="936" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A936" s="18"/>
+      <c r="B936" s="15"/>
+    </row>
+    <row r="937" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A937" s="18"/>
+      <c r="B937" s="15"/>
+    </row>
+    <row r="938" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A938" s="18"/>
+      <c r="B938" s="15"/>
+    </row>
+    <row r="939" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A939" s="18"/>
+      <c r="B939" s="15"/>
+    </row>
+    <row r="940" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A940" s="18"/>
+      <c r="B940" s="15"/>
+    </row>
+    <row r="941" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A941" s="18"/>
+      <c r="B941" s="15"/>
+    </row>
+    <row r="942" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A942" s="18"/>
+      <c r="B942" s="15"/>
+    </row>
+    <row r="943" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A943" s="18"/>
+      <c r="B943" s="15"/>
+    </row>
+    <row r="944" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A944" s="18"/>
+      <c r="B944" s="15"/>
+    </row>
+    <row r="945" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A945" s="18"/>
+      <c r="B945" s="15"/>
+    </row>
+    <row r="946" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A946" s="18"/>
+      <c r="B946" s="15"/>
+    </row>
+    <row r="947" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A947" s="18"/>
+      <c r="B947" s="15"/>
+    </row>
+    <row r="948" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A948" s="18"/>
+      <c r="B948" s="15"/>
+    </row>
+    <row r="949" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A949" s="18"/>
+      <c r="B949" s="15"/>
+    </row>
+    <row r="950" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A950" s="18"/>
+      <c r="B950" s="15"/>
+    </row>
+    <row r="951" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A951" s="18"/>
+      <c r="B951" s="15"/>
+    </row>
+    <row r="952" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A952" s="18"/>
+      <c r="B952" s="15"/>
+    </row>
+    <row r="953" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A953" s="18"/>
+      <c r="B953" s="15"/>
+    </row>
+    <row r="954" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A954" s="18"/>
+      <c r="B954" s="15"/>
+    </row>
+    <row r="955" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A955" s="18"/>
+      <c r="B955" s="15"/>
+    </row>
+    <row r="956" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A956" s="18"/>
+      <c r="B956" s="15"/>
+    </row>
+    <row r="957" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A957" s="18"/>
+      <c r="B957" s="15"/>
+    </row>
+    <row r="958" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A958" s="18"/>
+      <c r="B958" s="15"/>
+    </row>
+    <row r="959" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A959" s="18"/>
+      <c r="B959" s="15"/>
+    </row>
+    <row r="960" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A960" s="18"/>
+      <c r="B960" s="15"/>
+    </row>
+    <row r="961" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A961" s="18"/>
+      <c r="B961" s="15"/>
+    </row>
+    <row r="962" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A962" s="18"/>
+      <c r="B962" s="15"/>
+    </row>
+    <row r="963" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A963" s="18"/>
+      <c r="B963" s="15"/>
+    </row>
+    <row r="964" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A964" s="18"/>
+      <c r="B964" s="15"/>
+    </row>
+    <row r="965" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A965" s="18"/>
+      <c r="B965" s="15"/>
+    </row>
+    <row r="966" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A966" s="18"/>
+      <c r="B966" s="15"/>
+    </row>
+    <row r="967" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A967" s="18"/>
+      <c r="B967" s="15"/>
+    </row>
+    <row r="968" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A968" s="18"/>
+      <c r="B968" s="15"/>
+    </row>
+    <row r="969" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A969" s="18"/>
+      <c r="B969" s="15"/>
+    </row>
+    <row r="970" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A970" s="18"/>
+      <c r="B970" s="15"/>
+    </row>
+    <row r="971" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A971" s="18"/>
+      <c r="B971" s="15"/>
+    </row>
+    <row r="972" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A972" s="18"/>
+      <c r="B972" s="15"/>
+    </row>
+    <row r="973" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A973" s="18"/>
+      <c r="B973" s="15"/>
+    </row>
+    <row r="974" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A974" s="18"/>
+      <c r="B974" s="15"/>
+    </row>
+    <row r="975" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A975" s="18"/>
+      <c r="B975" s="15"/>
+    </row>
+    <row r="976" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A976" s="18"/>
+      <c r="B976" s="15"/>
+    </row>
+    <row r="977" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A977" s="18"/>
+      <c r="B977" s="15"/>
+    </row>
+    <row r="978" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A978" s="18"/>
+      <c r="B978" s="15"/>
+    </row>
+    <row r="979" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A979" s="18"/>
+      <c r="B979" s="15"/>
+    </row>
+    <row r="980" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A980" s="18"/>
+      <c r="B980" s="15"/>
+    </row>
+    <row r="981" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A981" s="18"/>
+      <c r="B981" s="15"/>
+    </row>
+    <row r="982" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A982" s="18"/>
+      <c r="B982" s="15"/>
+    </row>
+    <row r="983" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A983" s="18"/>
+      <c r="B983" s="15"/>
+    </row>
+    <row r="984" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A984" s="18"/>
+      <c r="B984" s="15"/>
+    </row>
+    <row r="985" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A985" s="18"/>
+      <c r="B985" s="15"/>
+    </row>
+    <row r="986" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A986" s="18"/>
+      <c r="B986" s="15"/>
+    </row>
+    <row r="987" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A987" s="18"/>
+      <c r="B987" s="15"/>
+    </row>
+    <row r="988" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A988" s="18"/>
+      <c r="B988" s="15"/>
+    </row>
+    <row r="989" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A989" s="18"/>
+      <c r="B989" s="15"/>
+    </row>
+    <row r="990" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A990" s="18"/>
+      <c r="B990" s="15"/>
+    </row>
+    <row r="991" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A991" s="18"/>
+      <c r="B991" s="15"/>
+    </row>
+    <row r="992" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A992" s="18"/>
+      <c r="B992" s="15"/>
+    </row>
+    <row r="993" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A993" s="18"/>
+      <c r="B993" s="15"/>
+    </row>
+    <row r="994" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A994" s="18"/>
+      <c r="B994" s="15"/>
+    </row>
+    <row r="995" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A995" s="18"/>
+      <c r="B995" s="15"/>
+    </row>
+    <row r="996" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A996" s="18"/>
+      <c r="B996" s="15"/>
+    </row>
+    <row r="997" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A997" s="18"/>
+      <c r="B997" s="15"/>
+    </row>
+    <row r="998" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A998" s="18"/>
+      <c r="B998" s="15"/>
+    </row>
+    <row r="999" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A999" s="18"/>
+      <c r="B999" s="15"/>
+    </row>
+    <row r="1000" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1000" s="18"/>
+      <c r="B1000" s="15"/>
+    </row>
+    <row r="1001" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1001" s="18"/>
+      <c r="B1001" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26D84380-F114-4A7F-B31E-FE519E05F99B}">
+  <sheetPr codeName="Sheet4">
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:Z1001"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="31.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="32" style="19" customWidth="1"/>
+    <col min="5" max="5" width="31" style="19" customWidth="1"/>
+    <col min="6" max="6" width="30.88671875" style="19" customWidth="1"/>
+    <col min="7" max="9" width="29.109375" style="19" customWidth="1"/>
+    <col min="10" max="16384" width="14.44140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+    </row>
+    <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+    </row>
+    <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32"/>
+      <c r="B4" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="37"/>
+    </row>
+    <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+    </row>
+    <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="37"/>
+    </row>
+    <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="29"/>
+      <c r="D9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+    </row>
+    <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="37"/>
+    </row>
+    <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+    </row>
+    <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+    </row>
+    <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+    </row>
+    <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>

</xml_diff>

<commit_message>
updated (committed wrongly prev) du for 7 Oct (Mon)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDB683E-9DDA-4A63-B609-D80092B2ACDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8A042B-9959-4085-8F43-D7F2AD1EFC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14296,9 +14296,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14396,10 +14396,10 @@
       <c r="B3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D3" s="37"/>
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -14411,10 +14411,10 @@
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D4" s="37"/>
       <c r="E4" s="29"/>
       <c r="F4" s="38"/>
       <c r="G4" s="38"/>
@@ -14426,10 +14426,10 @@
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="29" t="s">
         <v>35</v>
       </c>
+      <c r="D5" s="38"/>
       <c r="E5" s="29"/>
       <c r="F5" s="38"/>
       <c r="G5" s="38"/>
@@ -14443,10 +14443,10 @@
       <c r="B6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D6" s="37"/>
       <c r="E6" s="29"/>
       <c r="F6" s="38"/>
       <c r="G6" s="37"/>
@@ -14458,10 +14458,10 @@
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="29" t="s">
         <v>147</v>
       </c>
+      <c r="D7" s="38"/>
       <c r="E7" s="29"/>
       <c r="F7" s="37"/>
       <c r="G7" s="38"/>
@@ -14473,10 +14473,10 @@
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="29" t="s">
         <v>35</v>
       </c>
+      <c r="D8" s="38"/>
       <c r="E8" s="29"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -14490,10 +14490,10 @@
       <c r="B9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D9" s="37"/>
       <c r="E9" s="29"/>
       <c r="F9" s="38"/>
       <c r="G9" s="37"/>
@@ -14505,10 +14505,10 @@
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="10" t="s">
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D10" s="37"/>
       <c r="E10" s="29"/>
       <c r="F10" s="37"/>
       <c r="G10" s="38"/>
@@ -14520,10 +14520,10 @@
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29" t="s">
+      <c r="C11" s="29" t="s">
         <v>35</v>
       </c>
+      <c r="D11" s="38"/>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
@@ -14537,10 +14537,10 @@
       <c r="B12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D12" s="37"/>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
@@ -14552,10 +14552,10 @@
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="29" t="s">
         <v>146</v>
       </c>
+      <c r="D13" s="29"/>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -14567,10 +14567,10 @@
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="29" t="s">
         <v>35</v>
       </c>
+      <c r="D14" s="29"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -14584,10 +14584,10 @@
       <c r="B15" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29" t="s">
+      <c r="C15" s="29" t="s">
         <v>148</v>
       </c>
+      <c r="D15" s="29"/>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
       <c r="G15" s="37"/>
@@ -14599,10 +14599,10 @@
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="D16" s="10"/>
       <c r="E16" s="29"/>
       <c r="F16" s="37"/>
       <c r="G16" s="29"/>
@@ -14614,10 +14614,10 @@
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29" t="s">
+      <c r="C17" s="29" t="s">
         <v>35</v>
       </c>
+      <c r="D17" s="29"/>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>

</xml_diff>

<commit_message>
du for 8 Oct (Tues)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8A042B-9959-4085-8F43-D7F2AD1EFC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E439364-E43F-421F-BAC7-43F82CFE65A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14352" yWindow="3192" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="156">
   <si>
     <t>Question</t>
   </si>
@@ -479,6 +479,27 @@
   <si>
     <t>Updated the schedule</t>
   </si>
+  <si>
+    <t>Pair programming for starting &amp; clearing rounds with Lifu</t>
+  </si>
+  <si>
+    <t>Not clear about the requirement on starting &amp; clearing round. Require more understanding</t>
+  </si>
+  <si>
+    <t>Revise &amp; learn relevant php concepts and content to prepare for pair programming today</t>
+  </si>
+  <si>
+    <t>Pair programming for starting &amp; clearing rounds with tee yong</t>
+  </si>
+  <si>
+    <t>Hopefully not for the programming of clearing rounds</t>
+  </si>
+  <si>
+    <t>Revise on JSON and prepare some of the testcases</t>
+  </si>
+  <si>
+    <t>Not really sure how the out testcases syntax for bootstrap should be like</t>
+  </si>
 </sst>
 </file>
 
@@ -560,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -646,6 +667,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,12 +692,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -973,21 +997,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1007,8 +1031,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1073,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1074,7 +1098,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1121,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1120,7 +1144,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1145,7 +1169,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1168,7 +1192,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1191,7 +1215,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1216,7 +1240,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1239,7 +1263,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1262,7 +1286,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1287,7 +1311,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1310,7 +1334,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1357,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1358,7 +1382,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1381,7 +1405,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5380,21 +5404,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5414,8 +5438,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5456,7 +5480,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5485,7 +5509,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5512,7 +5536,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5539,7 +5563,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5568,7 +5592,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5595,7 +5619,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5622,7 +5646,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5651,7 +5675,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5678,7 +5702,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5705,7 +5729,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5734,7 +5758,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5761,7 +5785,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5788,7 +5812,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5817,7 +5841,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5844,7 +5868,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9847,21 +9871,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9881,8 +9905,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9923,7 +9947,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9952,7 +9976,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -9979,7 +10003,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10006,7 +10030,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10035,7 +10059,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10062,7 +10086,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10089,7 +10113,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10118,7 +10142,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10145,7 +10169,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10172,7 +10196,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10201,7 +10225,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10228,7 +10252,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10255,7 +10279,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10284,7 +10308,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10311,7 +10335,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14296,9 +14320,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E10" sqref="E10"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14314,21 +14338,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14348,8 +14372,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14390,7 +14414,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14399,7 +14423,9 @@
       <c r="C3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -14407,37 +14433,41 @@
       <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="32" t="s">
+        <v>149</v>
+      </c>
       <c r="E4" s="29"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="37"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="38"/>
+      <c r="D5" s="33" t="s">
+        <v>150</v>
+      </c>
       <c r="E5" s="29"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="34" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14446,45 +14476,51 @@
       <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="37"/>
+      <c r="D6" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="29"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="38"/>
+      <c r="D7" s="33" t="s">
+        <v>147</v>
+      </c>
       <c r="E7" s="29"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="37"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="38"/>
+      <c r="D8" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="29"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14493,37 +14529,43 @@
       <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="37"/>
+      <c r="D9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="E9" s="29"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="E10" s="29"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="37"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="38"/>
+      <c r="D11" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
@@ -14531,7 +14573,7 @@
       <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="34" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14540,7 +14582,9 @@
       <c r="C12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="37"/>
+      <c r="D12" s="32" t="s">
+        <v>151</v>
+      </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
@@ -14548,29 +14592,33 @@
       <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
+      <c r="A13" s="35"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="31" t="s">
+        <v>152</v>
+      </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
-      <c r="I13" s="37"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="31" t="s">
+        <v>153</v>
+      </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -14578,7 +14626,7 @@
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="34" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14587,37 +14635,43 @@
       <c r="C15" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="37"/>
+      <c r="G15" s="32"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
+      <c r="A16" s="35"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="32" t="s">
+        <v>154</v>
+      </c>
       <c r="E16" s="29"/>
-      <c r="F16" s="37"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="29" t="s">
+        <v>155</v>
+      </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>

</xml_diff>

<commit_message>
uodated du for 8 Oct (Tues) (made a mistake for prev one)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E439364-E43F-421F-BAC7-43F82CFE65A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A54781-1125-40F8-97CE-307FC8254A75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14352" yWindow="3192" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="158">
   <si>
     <t>Question</t>
   </si>
@@ -499,6 +499,12 @@
   </si>
   <si>
     <t>Not really sure how the out testcases syntax for bootstrap should be like</t>
+  </si>
+  <si>
+    <t>Continue to finish the makebid.php + validation</t>
+  </si>
+  <si>
+    <t>Trying to figure out and troubleshoot why my code doesn’t work</t>
   </si>
 </sst>
 </file>
@@ -14320,9 +14326,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D18" sqref="D18"/>
+      <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14546,8 +14552,8 @@
       <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>31</v>
+      <c r="D10" s="32" t="s">
+        <v>156</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="32"/>
@@ -14564,7 +14570,7 @@
         <v>35</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>35</v>
+        <v>157</v>
       </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>

</xml_diff>

<commit_message>
du for 9 Oct (Wed)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A54781-1125-40F8-97CE-307FC8254A75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF3027-D329-4312-AB28-E86D0F8404F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="164">
   <si>
     <t>Question</t>
   </si>
@@ -506,6 +506,24 @@
   <si>
     <t>Trying to figure out and troubleshoot why my code doesn’t work</t>
   </si>
+  <si>
+    <t>Pair programming and finished makebid.php + validation with Yu Liang</t>
+  </si>
+  <si>
+    <t>Pair programming and finished makebid.php + validation with Christine</t>
+  </si>
+  <si>
+    <t>Look at the requirement of delete and edit bid</t>
+  </si>
+  <si>
+    <t>Pair programming for starting &amp; clearing rounds with Tee Yong</t>
+  </si>
+  <si>
+    <t>Preparation of testcases for JSON</t>
+  </si>
+  <si>
+    <t>Troubleshooting and pair the codes with Yu Liang's</t>
+  </si>
 </sst>
 </file>
 
@@ -587,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -680,6 +698,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1003,21 +1024,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1037,8 +1058,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1079,7 +1100,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1104,7 +1125,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1127,7 +1148,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1171,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1175,7 +1196,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1198,7 +1219,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1221,7 +1242,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1246,7 +1267,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1269,7 +1290,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1292,7 +1313,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1317,7 +1338,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1340,7 +1361,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1363,7 +1384,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1388,7 +1409,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1411,7 +1432,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5410,21 +5431,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5444,8 +5465,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5486,7 +5507,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5515,7 +5536,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5542,7 +5563,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5569,7 +5590,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5598,7 +5619,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5625,7 +5646,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5652,7 +5673,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5681,7 +5702,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5708,7 +5729,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5735,7 +5756,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5764,7 +5785,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5791,7 +5812,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5818,7 +5839,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5847,7 +5868,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5874,7 +5895,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9877,21 +9898,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9911,8 +9932,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9953,7 +9974,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -9982,7 +10003,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -10009,7 +10030,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10036,7 +10057,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10065,7 +10086,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10092,7 +10113,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10119,7 +10140,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10148,7 +10169,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10175,7 +10196,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10202,7 +10223,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10231,7 +10252,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10258,7 +10279,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10285,7 +10306,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10314,7 +10335,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10341,7 +10362,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14326,9 +14347,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14344,21 +14365,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14378,8 +14399,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14420,7 +14441,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="35" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14432,14 +14453,16 @@
       <c r="D3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="29"/>
+      <c r="E3" s="34" t="s">
+        <v>149</v>
+      </c>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
@@ -14449,14 +14472,16 @@
       <c r="D4" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
@@ -14466,14 +14491,16 @@
       <c r="D5" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="35" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14485,14 +14512,16 @@
       <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="34" t="s">
+        <v>158</v>
+      </c>
       <c r="F6" s="33"/>
       <c r="G6" s="32"/>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
@@ -14500,16 +14529,18 @@
         <v>147</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="29"/>
+        <v>156</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F7" s="32"/>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
@@ -14517,16 +14548,18 @@
         <v>35</v>
       </c>
       <c r="D8" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="29"/>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14538,14 +14571,16 @@
       <c r="D9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="29"/>
+      <c r="E9" s="34" t="s">
+        <v>159</v>
+      </c>
       <c r="F9" s="33"/>
       <c r="G9" s="32"/>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
@@ -14555,14 +14590,16 @@
       <c r="D10" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="34" t="s">
+        <v>160</v>
+      </c>
       <c r="F10" s="32"/>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
       <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
@@ -14572,14 +14609,16 @@
       <c r="D11" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="29"/>
+      <c r="E11" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="35" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14591,14 +14630,16 @@
       <c r="D12" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="29"/>
+      <c r="E12" s="34" t="s">
+        <v>161</v>
+      </c>
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -14608,14 +14649,16 @@
       <c r="D13" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -14625,14 +14668,16 @@
       <c r="D14" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14644,14 +14689,16 @@
       <c r="D15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>162</v>
+      </c>
       <c r="F15" s="29"/>
       <c r="G15" s="32"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
+      <c r="A16" s="36"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
@@ -14661,14 +14708,16 @@
       <c r="D16" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="F16" s="32"/>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
@@ -14678,7 +14727,9 @@
       <c r="D17" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="E17" s="29"/>
+      <c r="E17" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="F17" s="29"/>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>

</xml_diff>

<commit_message>
du for 10 Oct (Thurs)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DF3027-D329-4312-AB28-E86D0F8404F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D816C-9D04-41EF-9A4A-3A6D5D8FDA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="171">
   <si>
     <t>Question</t>
   </si>
@@ -524,6 +524,27 @@
   <si>
     <t>Troubleshooting and pair the codes with Yu Liang's</t>
   </si>
+  <si>
+    <t>Build test cases for start / clear rounds, debug wherever necessary, continue the development of rounds clearing through pair programming with tee yong, create &amp; update test cases with teammates and schedule debug with tee yong if needed</t>
+  </si>
+  <si>
+    <t>having trouble understanding json requirements</t>
+  </si>
+  <si>
+    <t>Create test cases for start / clear rounds, continue the development of rounds clearing through pair programming with lifu.</t>
+  </si>
+  <si>
+    <t>Look at the requirement of delete and edit bid, draft out the logic</t>
+  </si>
+  <si>
+    <t>Work on JSON with Wang Ting</t>
+  </si>
+  <si>
+    <t>Work on JSON with Christine</t>
+  </si>
+  <si>
+    <t>Finding out the optimal way of doing the testcases for the JSON (it was not as straight forward as I thought)</t>
+  </si>
 </sst>
 </file>
 
@@ -605,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -698,6 +719,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1024,21 +1048,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1058,8 +1082,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1100,7 +1124,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1125,7 +1149,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1148,7 +1172,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1195,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1196,7 +1220,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1243,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1242,7 +1266,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1267,7 +1291,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1290,7 +1314,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1313,7 +1337,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1338,7 +1362,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1361,7 +1385,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1384,7 +1408,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1409,7 +1433,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1432,7 +1456,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5431,21 +5455,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5465,8 +5489,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5507,7 +5531,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5536,7 +5560,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5563,7 +5587,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5590,7 +5614,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5619,7 +5643,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5646,7 +5670,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5673,7 +5697,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5702,7 +5726,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5729,7 +5753,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5756,7 +5780,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5785,7 +5809,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5812,7 +5836,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5839,7 +5863,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5868,7 +5892,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5895,7 +5919,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9898,21 +9922,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9932,8 +9956,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9974,7 +9998,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -10003,7 +10027,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -10030,7 +10054,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10057,7 +10081,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10086,7 +10110,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10113,7 +10137,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10140,7 +10164,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10169,7 +10193,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10196,7 +10220,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10223,7 +10247,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10252,7 +10276,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10279,7 +10303,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10306,7 +10330,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10335,7 +10359,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10362,7 +10386,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14347,9 +14371,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14365,21 +14389,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14399,8 +14423,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14441,7 +14465,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14456,13 +14480,15 @@
       <c r="E3" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="29"/>
+      <c r="F3" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
@@ -14475,13 +14501,15 @@
       <c r="E4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="33" t="s">
+        <v>166</v>
+      </c>
       <c r="G4" s="33"/>
       <c r="H4" s="33"/>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
@@ -14494,13 +14522,15 @@
       <c r="E5" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="36" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14515,13 +14545,15 @@
       <c r="E6" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="33" t="s">
+        <v>167</v>
+      </c>
       <c r="G6" s="32"/>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
@@ -14534,13 +14566,15 @@
       <c r="E7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="32" t="s">
+        <v>168</v>
+      </c>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
@@ -14553,13 +14587,15 @@
       <c r="E8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" s="33"/>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14574,13 +14610,15 @@
       <c r="E9" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="33" t="s">
+        <v>160</v>
+      </c>
       <c r="G9" s="32"/>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
@@ -14593,13 +14631,15 @@
       <c r="E10" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G10" s="33"/>
       <c r="H10" s="33"/>
       <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
@@ -14612,13 +14652,15 @@
       <c r="E11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="29"/>
+      <c r="F11" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="G11" s="29"/>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14633,13 +14675,15 @@
       <c r="E12" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G12" s="29"/>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -14652,13 +14696,15 @@
       <c r="E13" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="35" t="s">
+        <v>164</v>
+      </c>
       <c r="G13" s="29"/>
       <c r="H13" s="29"/>
       <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
+      <c r="A14" s="37"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -14671,13 +14717,15 @@
       <c r="E14" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="35" t="s">
+        <v>165</v>
+      </c>
       <c r="G14" s="29"/>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14692,13 +14740,15 @@
       <c r="E15" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="F15" s="29"/>
+      <c r="F15" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="G15" s="32"/>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
@@ -14711,13 +14761,15 @@
       <c r="E16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="32"/>
+      <c r="F16" s="32" t="s">
+        <v>169</v>
+      </c>
       <c r="G16" s="29"/>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
@@ -14730,7 +14782,9 @@
       <c r="E17" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="29" t="s">
+        <v>170</v>
+      </c>
       <c r="G17" s="29"/>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>

</xml_diff>

<commit_message>
du for 11 Oct (Fri)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D816C-9D04-41EF-9A4A-3A6D5D8FDA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A210838D-61B9-4A1D-AC7B-4175E6C7883A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="184">
   <si>
     <t>Question</t>
   </si>
@@ -545,6 +545,45 @@
   <si>
     <t>Finding out the optimal way of doing the testcases for the JSON (it was not as straight forward as I thought)</t>
   </si>
+  <si>
+    <t>Debugging &amp; pair programming for rounds clearing with tee yong</t>
+  </si>
+  <si>
+    <t>Continue working on rounds clearing with tee yong, test teammates' edit &amp; drop bid function and update the documentation accordingly</t>
+  </si>
+  <si>
+    <t>Figuring out what causes a code to loop infinitely during the development of rounds clearing</t>
+  </si>
+  <si>
+    <t>Pair programming with Wangting for JSON authentication. Prepare authentication test cases and testing of Start &amp; Clear Rounds by Lifu and TeeYong.</t>
+  </si>
+  <si>
+    <t>Continue pair programming and prepare test cases for bootstrap. Push edit &amp; drop bid functions with Yu Liang.</t>
+  </si>
+  <si>
+    <t>Figure out why the e dollar keeps getting updated wrongly</t>
+  </si>
+  <si>
+    <t>Debugging &amp; pair programming for rounds clearing with lifu</t>
+  </si>
+  <si>
+    <t>Continue working on rounds clearing with lifu, test teammates' edit &amp; drop bid function and update the documentation accordingly</t>
+  </si>
+  <si>
+    <t>error in code causing infinite loop</t>
+  </si>
+  <si>
+    <t>Continue pair programming and prepare test cases for bootstrap. Push edit &amp; drop bid functions with Christine</t>
+  </si>
+  <si>
+    <t>Pair Programming with Christine for JSON authentication. Prepared the authentication test cases and did testing of Start and Clear Rounds (done by Lifu and Tee Yong)</t>
+  </si>
+  <si>
+    <t>Pair Programming with Christine today on JSON bootstrap and prepare the test cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scheduling as everyone have commitments so it is hard to fulfil the functions we originally intended / the tasks are taking longer than planned to be completed. </t>
+  </si>
 </sst>
 </file>
 
@@ -626,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -719,6 +758,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1048,21 +1090,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1082,8 +1124,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1124,7 +1166,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1149,7 +1191,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1214,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1195,7 +1237,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1220,7 +1262,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1243,7 +1285,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1266,7 +1308,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1291,7 +1333,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1314,7 +1356,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1379,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1362,7 +1404,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1385,7 +1427,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1408,7 +1450,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1433,7 +1475,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1456,7 +1498,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5455,21 +5497,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5489,8 +5531,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5531,7 +5573,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5560,7 +5602,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5587,7 +5629,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5614,7 +5656,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5643,7 +5685,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5670,7 +5712,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5697,7 +5739,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5726,7 +5768,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5753,7 +5795,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5780,7 +5822,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5809,7 +5851,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5836,7 +5878,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5863,7 +5905,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5892,7 +5934,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5919,7 +5961,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9922,21 +9964,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9956,8 +9998,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -9998,7 +10040,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -10027,7 +10069,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -10054,7 +10096,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10081,7 +10123,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10110,7 +10152,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10137,7 +10179,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10164,7 +10206,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10193,7 +10235,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10220,7 +10262,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10247,7 +10289,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10276,7 +10318,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10303,7 +10345,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10330,7 +10372,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10359,7 +10401,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10386,7 +10428,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14371,9 +14413,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14389,21 +14431,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14423,8 +14465,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14465,7 +14507,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="37" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14483,12 +14525,14 @@
       <c r="F3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="36" t="s">
+        <v>177</v>
+      </c>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
@@ -14504,12 +14548,14 @@
       <c r="F4" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="33"/>
+      <c r="G4" s="33" t="s">
+        <v>178</v>
+      </c>
       <c r="H4" s="33"/>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
@@ -14525,12 +14571,14 @@
       <c r="F5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="33" t="s">
+        <v>179</v>
+      </c>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14548,12 +14596,14 @@
       <c r="F6" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="G6" s="32"/>
+      <c r="G6" s="32" t="s">
+        <v>174</v>
+      </c>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
@@ -14569,12 +14619,14 @@
       <c r="F7" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="G7" s="33"/>
+      <c r="G7" s="33" t="s">
+        <v>175</v>
+      </c>
       <c r="H7" s="33"/>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
@@ -14590,12 +14642,14 @@
       <c r="F8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="33"/>
+      <c r="G8" s="33" t="s">
+        <v>176</v>
+      </c>
       <c r="H8" s="33"/>
       <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="37" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14613,12 +14667,14 @@
       <c r="F9" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="10" t="s">
+        <v>31</v>
+      </c>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
@@ -14634,12 +14690,14 @@
       <c r="F10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="33"/>
+      <c r="G10" s="33" t="s">
+        <v>180</v>
+      </c>
       <c r="H10" s="33"/>
       <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
@@ -14655,12 +14713,14 @@
       <c r="F11" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="29"/>
+      <c r="G11" s="36" t="s">
+        <v>176</v>
+      </c>
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="37" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14678,12 +14738,14 @@
       <c r="F12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="36" t="s">
+        <v>171</v>
+      </c>
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -14699,12 +14761,14 @@
       <c r="F13" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="36" t="s">
+        <v>172</v>
+      </c>
       <c r="H13" s="29"/>
       <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -14720,12 +14784,14 @@
       <c r="F14" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="36" t="s">
+        <v>173</v>
+      </c>
       <c r="H14" s="29"/>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14743,12 +14809,14 @@
       <c r="F15" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="32"/>
+      <c r="G15" s="32" t="s">
+        <v>181</v>
+      </c>
       <c r="H15" s="29"/>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="37"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
@@ -14764,12 +14832,14 @@
       <c r="F16" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="G16" s="29"/>
+      <c r="G16" s="29" t="s">
+        <v>182</v>
+      </c>
       <c r="H16" s="29"/>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="37"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
@@ -14785,7 +14855,9 @@
       <c r="F17" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="G17" s="29"/>
+      <c r="G17" s="29" t="s">
+        <v>183</v>
+      </c>
       <c r="H17" s="29"/>
       <c r="I17" s="29"/>
     </row>

</xml_diff>

<commit_message>
du for 12 Oct (Sat)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A210838D-61B9-4A1D-AC7B-4175E6C7883A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A74EEA3-E9A8-4843-B1C0-9CF5A06CF2DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="194">
   <si>
     <t>Question</t>
   </si>
@@ -583,6 +583,36 @@
   </si>
   <si>
     <t xml:space="preserve">Scheduling as everyone have commitments so it is hard to fulfil the functions we originally intended / the tasks are taking longer than planned to be completed. </t>
+  </si>
+  <si>
+    <t>Help to do validation for edit bid with Christine</t>
+  </si>
+  <si>
+    <t>Didn't pull in github for a while which resulted in some clashes between different php files when I'm trying to commit and push codes</t>
+  </si>
+  <si>
+    <t>Pair programming for clearing rounds with tee yong</t>
+  </si>
+  <si>
+    <t>continue pair programming for clearing round with tee yong</t>
+  </si>
+  <si>
+    <t>Fix bug of missing validations for edit bid with Yu Liang. Test rounds clearing after they are complete.</t>
+  </si>
+  <si>
+    <t>Code conflicts between GET and POST method</t>
+  </si>
+  <si>
+    <t>Pair programming for clearing rounds with lifu</t>
+  </si>
+  <si>
+    <t>continue pair programming for clearing round with lifu</t>
+  </si>
+  <si>
+    <t>Pair Programming with Christine on JSON Bootstrap, prepared testcases and did testing, minor adjustment to Bootstrap.php</t>
+  </si>
+  <si>
+    <t>Scheduling</t>
   </si>
 </sst>
 </file>
@@ -665,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -758,6 +788,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1090,21 +1123,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1124,8 +1157,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1166,7 +1199,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1191,7 +1224,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1214,7 +1247,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1237,7 +1270,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1262,7 +1295,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1285,7 +1318,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1341,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1333,7 +1366,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1389,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1379,7 +1412,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1404,7 +1437,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1427,7 +1460,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1450,7 +1483,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1475,7 +1508,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1498,7 +1531,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5497,21 +5530,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5531,8 +5564,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5573,7 +5606,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5602,7 +5635,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5629,7 +5662,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5656,7 +5689,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5685,7 +5718,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5712,7 +5745,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5739,7 +5772,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5768,7 +5801,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5795,7 +5828,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5822,7 +5855,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5851,7 +5884,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5878,7 +5911,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5905,7 +5938,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5934,7 +5967,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5961,7 +5994,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9964,21 +9997,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -9998,8 +10031,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -10040,7 +10073,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -10069,7 +10102,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -10096,7 +10129,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10123,7 +10156,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10152,7 +10185,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10179,7 +10212,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10206,7 +10239,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10235,7 +10268,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10262,7 +10295,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10289,7 +10322,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10318,7 +10351,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10345,7 +10378,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10372,7 +10405,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10401,7 +10434,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10428,7 +10461,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14413,9 +14446,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G17" sqref="G17"/>
+      <selection pane="topRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14431,21 +14464,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14465,8 +14498,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14507,7 +14540,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="38" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14528,11 +14561,13 @@
       <c r="G3" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="H3" s="29"/>
+      <c r="H3" s="37" t="s">
+        <v>190</v>
+      </c>
       <c r="I3" s="29"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
@@ -14551,11 +14586,13 @@
       <c r="G4" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="H4" s="33"/>
+      <c r="H4" s="33" t="s">
+        <v>191</v>
+      </c>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
@@ -14574,11 +14611,13 @@
       <c r="G5" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="H5" s="33"/>
+      <c r="H5" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14599,11 +14638,13 @@
       <c r="G6" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="H6" s="33"/>
+      <c r="H6" s="33" t="s">
+        <v>175</v>
+      </c>
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
@@ -14622,11 +14663,13 @@
       <c r="G7" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="H7" s="33"/>
+      <c r="H7" s="33" t="s">
+        <v>188</v>
+      </c>
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
@@ -14645,11 +14688,13 @@
       <c r="G8" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="H8" s="33"/>
+      <c r="H8" s="33" t="s">
+        <v>189</v>
+      </c>
       <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="38" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14670,11 +14715,13 @@
       <c r="G9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="33"/>
+      <c r="H9" s="33" t="s">
+        <v>180</v>
+      </c>
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
@@ -14693,11 +14740,13 @@
       <c r="G10" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="H10" s="33"/>
+      <c r="H10" s="33" t="s">
+        <v>184</v>
+      </c>
       <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
@@ -14716,11 +14765,13 @@
       <c r="G11" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="H11" s="29"/>
+      <c r="H11" s="37" t="s">
+        <v>185</v>
+      </c>
       <c r="I11" s="29"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="38" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14741,11 +14792,13 @@
       <c r="G12" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="H12" s="29"/>
+      <c r="H12" s="37" t="s">
+        <v>186</v>
+      </c>
       <c r="I12" s="29"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -14764,11 +14817,13 @@
       <c r="G13" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="H13" s="29"/>
+      <c r="H13" s="33" t="s">
+        <v>187</v>
+      </c>
       <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -14787,11 +14842,13 @@
       <c r="G14" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="H14" s="29"/>
+      <c r="H14" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14812,11 +14869,13 @@
       <c r="G15" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="29"/>
+      <c r="H15" s="29" t="s">
+        <v>192</v>
+      </c>
       <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
@@ -14835,11 +14894,13 @@
       <c r="G16" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29" t="s">
+        <v>193</v>
+      </c>
       <c r="I16" s="29"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
@@ -14858,7 +14919,9 @@
       <c r="G17" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="H17" s="29"/>
+      <c r="H17" s="29" t="s">
+        <v>35</v>
+      </c>
       <c r="I17" s="29"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
du for 13 Oct (Sun)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A74EEA3-E9A8-4843-B1C0-9CF5A06CF2DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A10E41-27E2-4DE6-9DDA-A552A4CCDAC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6552" yWindow="1152" windowWidth="23016" windowHeight="12336" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="201">
   <si>
     <t>Question</t>
   </si>
@@ -613,6 +613,27 @@
   </si>
   <si>
     <t>Scheduling</t>
+  </si>
+  <si>
+    <t>pair programming with tee yong for view bidding results &amp; meeting with team to do final testing &amp; deployment</t>
+  </si>
+  <si>
+    <t>navigating between all the DAOs to figure out the cause of errors for my code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pair Programming with Christine on JSON, meeting with the team to do final testing and deployment, prepare for App Demo </t>
+  </si>
+  <si>
+    <t>Fixed bug of missing validations for edit bid with Yu Liang. Tested rounds clearing after they are complete.</t>
+  </si>
+  <si>
+    <t>Meeting with team to do final testing &amp; deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet up with up with the team to do final testing and deployment </t>
+  </si>
+  <si>
+    <t>pair programming with lifu for view bidding results. Attend team meeting to do final testing &amp; deployment</t>
   </si>
 </sst>
 </file>
@@ -695,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -788,6 +809,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1123,21 +1147,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1157,8 +1181,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1199,7 +1223,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1224,7 +1248,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1247,7 +1271,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1294,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1295,7 +1319,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1318,7 +1342,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1341,7 +1365,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1366,7 +1390,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1389,7 +1413,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1412,7 +1436,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1437,7 +1461,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1460,7 +1484,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1483,7 +1507,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1508,7 +1532,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1531,7 +1555,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5530,21 +5554,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5564,8 +5588,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5606,7 +5630,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5635,7 +5659,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5662,7 +5686,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5689,7 +5713,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5718,7 +5742,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5745,7 +5769,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5772,7 +5796,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5801,7 +5825,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5828,7 +5852,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5855,7 +5879,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5884,7 +5908,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5911,7 +5935,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -5938,7 +5962,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -5967,7 +5991,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -5994,7 +6018,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -9997,21 +10021,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -10031,8 +10055,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -10073,7 +10097,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -10102,7 +10126,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -10129,7 +10153,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10156,7 +10180,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10185,7 +10209,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10212,7 +10236,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10239,7 +10263,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10268,7 +10292,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10295,7 +10319,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10322,7 +10346,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10351,7 +10375,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10378,7 +10402,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10405,7 +10429,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10434,7 +10458,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10461,7 +10485,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14446,9 +14470,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14464,21 +14488,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14498,8 +14522,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14540,7 +14564,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="39" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14564,10 +14588,12 @@
       <c r="H3" s="37" t="s">
         <v>190</v>
       </c>
-      <c r="I3" s="29"/>
+      <c r="I3" s="38" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="40"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
@@ -14589,10 +14615,12 @@
       <c r="H4" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="I4" s="32"/>
+      <c r="I4" s="32" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
@@ -14614,10 +14642,12 @@
       <c r="H5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="33"/>
+      <c r="I5" s="33" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14641,10 +14671,12 @@
       <c r="H6" s="33" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="33" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
@@ -14666,10 +14698,12 @@
       <c r="H7" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="32" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="40"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
@@ -14691,10 +14725,12 @@
       <c r="H8" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="I8" s="33"/>
+      <c r="I8" s="33" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14718,10 +14754,12 @@
       <c r="H9" s="33" t="s">
         <v>180</v>
       </c>
-      <c r="I9" s="33"/>
+      <c r="I9" s="33" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
@@ -14743,10 +14781,12 @@
       <c r="H10" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="I10" s="32"/>
+      <c r="I10" s="32" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
@@ -14768,10 +14808,12 @@
       <c r="H11" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="I11" s="29"/>
+      <c r="I11" s="29" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="39" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14795,10 +14837,12 @@
       <c r="H12" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="I12" s="29"/>
+      <c r="I12" s="38" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -14820,10 +14864,12 @@
       <c r="H13" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="I13" s="32"/>
+      <c r="I13" s="32" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
+      <c r="A14" s="40"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -14845,10 +14891,12 @@
       <c r="H14" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="29"/>
+      <c r="I14" s="38" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="39" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14872,10 +14920,12 @@
       <c r="H15" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="I15" s="29"/>
+      <c r="I15" s="29" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
@@ -14897,10 +14947,12 @@
       <c r="H16" s="29" t="s">
         <v>193</v>
       </c>
-      <c r="I16" s="29"/>
+      <c r="I16" s="29" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
@@ -14922,7 +14974,9 @@
       <c r="H17" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="29"/>
+      <c r="I17" s="29" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>

</xml_diff>

<commit_message>
du for 15 Oct (Tues)
</commit_message>
<xml_diff>
--- a/metrics/du.xlsx
+++ b/metrics/du.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\project-g8t9\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1FE2F7-461E-42F8-82EC-98A788D79172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13003844-9356-4745-8CEF-8C42057E532C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="-204" windowWidth="23016" windowHeight="12336" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 5" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="216">
   <si>
     <t>Question</t>
   </si>
@@ -666,6 +666,21 @@
   <si>
     <t>Meet up with up with the team to do final testing and deployment</t>
   </si>
+  <si>
+    <t>resolved bug found in our website while testing.</t>
+  </si>
+  <si>
+    <t>Debug with teeyong and deploy with PM at night</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further testing and deployment </t>
+  </si>
+  <si>
+    <t>App Demo and team meeting</t>
+  </si>
+  <si>
+    <t>App Demo and Team Meeting</t>
+  </si>
 </sst>
 </file>
 
@@ -863,6 +878,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -879,9 +897,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1187,21 +1202,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1221,8 +1236,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1263,7 +1278,7 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -1288,7 +1303,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
@@ -1311,7 +1326,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1334,7 +1349,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1359,7 +1374,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1382,7 +1397,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1405,7 +1420,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1430,7 +1445,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1453,7 +1468,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1476,7 +1491,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1501,7 +1516,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1524,7 +1539,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1547,7 +1562,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1572,7 +1587,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="8" t="s">
         <v>8</v>
       </c>
@@ -1595,7 +1610,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
@@ -5594,21 +5609,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -5628,8 +5643,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
@@ -5670,7 +5685,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -5699,7 +5714,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
@@ -5726,7 +5741,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
@@ -5753,7 +5768,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -5782,7 +5797,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="12" t="s">
         <v>8</v>
       </c>
@@ -5809,7 +5824,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
@@ -5836,7 +5851,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -5865,7 +5880,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
       </c>
@@ -5892,7 +5907,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
@@ -5919,7 +5934,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -5948,7 +5963,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="12" t="s">
         <v>8</v>
       </c>
@@ -5975,7 +5990,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
@@ -6002,7 +6017,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -6031,7 +6046,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
@@ -6058,7 +6073,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
@@ -10061,21 +10076,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -10095,8 +10110,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="22" t="s">
         <v>2</v>
       </c>
@@ -10137,7 +10152,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -10166,7 +10181,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -10193,7 +10208,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="20" t="s">
         <v>9</v>
       </c>
@@ -10220,7 +10235,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -10249,7 +10264,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="20" t="s">
         <v>8</v>
       </c>
@@ -10276,7 +10291,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="20" t="s">
         <v>9</v>
       </c>
@@ -10303,7 +10318,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -10332,7 +10347,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
@@ -10359,7 +10374,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
@@ -10386,7 +10401,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -10415,7 +10430,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
@@ -10442,7 +10457,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="20" t="s">
         <v>9</v>
       </c>
@@ -10469,7 +10484,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -10498,7 +10513,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="20" t="s">
         <v>8</v>
       </c>
@@ -10525,7 +10540,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
@@ -14528,21 +14543,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -14562,8 +14577,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="30" t="s">
         <v>2</v>
       </c>
@@ -14604,7 +14619,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="28" t="s">
@@ -14633,7 +14648,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="28" t="s">
         <v>12</v>
       </c>
@@ -14660,7 +14675,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="28" t="s">
         <v>9</v>
       </c>
@@ -14687,7 +14702,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="28" t="s">
@@ -14716,7 +14731,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="28" t="s">
         <v>8</v>
       </c>
@@ -14743,7 +14758,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="28" t="s">
         <v>9</v>
       </c>
@@ -14770,7 +14785,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="28" t="s">
@@ -14799,7 +14814,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="28" t="s">
         <v>8</v>
       </c>
@@ -14826,7 +14841,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="28" t="s">
         <v>9</v>
       </c>
@@ -14853,7 +14868,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="28" t="s">
@@ -14882,7 +14897,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="28" t="s">
         <v>8</v>
       </c>
@@ -14909,7 +14924,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
@@ -14936,7 +14951,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="28" t="s">
@@ -14965,7 +14980,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="28" t="s">
         <v>8</v>
       </c>
@@ -14992,7 +15007,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
@@ -18977,9 +18992,9 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C15" sqref="C15"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18995,21 +19010,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -19029,8 +19044,8 @@
       <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="40" t="s">
         <v>2</v>
       </c>
@@ -19071,7 +19086,7 @@
       <c r="Z2" s="18"/>
     </row>
     <row r="3" spans="1:26" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="42" t="s">
         <v>57</v>
       </c>
       <c r="B3" s="39" t="s">
@@ -19080,7 +19095,9 @@
       <c r="C3" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="32" t="s">
+        <v>211</v>
+      </c>
       <c r="E3" s="33"/>
       <c r="F3" s="32"/>
       <c r="G3" s="33"/>
@@ -19088,14 +19105,16 @@
       <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
+      <c r="A4" s="43"/>
       <c r="B4" s="39" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="32" t="s">
+        <v>214</v>
+      </c>
       <c r="E4" s="32"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
@@ -19103,14 +19122,16 @@
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
@@ -19118,7 +19139,7 @@
       <c r="I5" s="33"/>
     </row>
     <row r="6" spans="1:26" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="39" t="s">
@@ -19127,7 +19148,9 @@
       <c r="C6" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="32" t="s">
+        <v>204</v>
+      </c>
       <c r="E6" s="33"/>
       <c r="F6" s="33"/>
       <c r="G6" s="32"/>
@@ -19135,14 +19158,16 @@
       <c r="I6" s="33"/>
     </row>
     <row r="7" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="39" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="33" t="s">
+        <v>214</v>
+      </c>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
       <c r="G7" s="33"/>
@@ -19150,14 +19175,16 @@
       <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E8" s="33"/>
       <c r="F8" s="33"/>
       <c r="G8" s="33"/>
@@ -19165,7 +19192,7 @@
       <c r="I8" s="33"/>
     </row>
     <row r="9" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="39" t="s">
@@ -19174,7 +19201,9 @@
       <c r="C9" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="32" t="s">
+        <v>204</v>
+      </c>
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
       <c r="G9" s="32"/>
@@ -19182,14 +19211,16 @@
       <c r="I9" s="33"/>
     </row>
     <row r="10" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="39" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="32" t="s">
+        <v>214</v>
+      </c>
       <c r="E10" s="33"/>
       <c r="F10" s="32"/>
       <c r="G10" s="33"/>
@@ -19197,14 +19228,16 @@
       <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="43"/>
       <c r="B11" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
@@ -19212,7 +19245,7 @@
       <c r="I11" s="33"/>
     </row>
     <row r="12" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="42" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="39" t="s">
@@ -19221,7 +19254,9 @@
       <c r="C12" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="32"/>
+      <c r="D12" s="32" t="s">
+        <v>212</v>
+      </c>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
@@ -19229,14 +19264,16 @@
       <c r="I12" s="33"/>
     </row>
     <row r="13" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42"/>
+      <c r="A13" s="43"/>
       <c r="B13" s="39" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="D13" s="33"/>
+      <c r="D13" s="33" t="s">
+        <v>214</v>
+      </c>
       <c r="E13" s="32"/>
       <c r="F13" s="33"/>
       <c r="G13" s="33"/>
@@ -19244,14 +19281,16 @@
       <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="33"/>
+      <c r="D14" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
       <c r="G14" s="33"/>
@@ -19259,7 +19298,7 @@
       <c r="I14" s="33"/>
     </row>
     <row r="15" spans="1:26" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="42" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="39" t="s">
@@ -19268,7 +19307,9 @@
       <c r="C15" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="D15" s="32"/>
+      <c r="D15" s="32" t="s">
+        <v>213</v>
+      </c>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
@@ -19276,14 +19317,16 @@
       <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:26" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="42"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="39" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="D16" s="32"/>
+      <c r="D16" s="32" t="s">
+        <v>215</v>
+      </c>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -19291,14 +19334,16 @@
       <c r="I16" s="33"/>
     </row>
     <row r="17" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="33"/>
+      <c r="D17" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="E17" s="33"/>
       <c r="F17" s="33"/>
       <c r="G17" s="33"/>
@@ -19308,13 +19353,13 @@
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>

</xml_diff>